<commit_message>
Python cheat sheet version 1.2 by Acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acopt\Desktop\My-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614E7578-A432-401D-B3D0-8FF7E494E45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7DD949-5CA5-45A4-996A-C2BE6F8A19A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="232">
   <si>
     <t>Data Conversion</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>for i in list:</t>
-  </si>
-  <si>
-    <t>draw.io</t>
   </si>
   <si>
     <t>immutable</t>
@@ -651,24 +648,15 @@
     </r>
   </si>
   <si>
-    <t>devdocs.io</t>
-  </si>
-  <si>
     <t>Lists</t>
   </si>
   <si>
     <t>Collections</t>
   </si>
   <si>
-    <t>HTML</t>
-  </si>
-  <si>
     <t>Python</t>
   </si>
   <si>
-    <t>HTML,CSS and others</t>
-  </si>
-  <si>
     <t>"""  """ docstrings</t>
   </si>
   <si>
@@ -709,13 +697,109 @@
   </si>
   <si>
     <t>type(element)-returns the type of element</t>
+  </si>
+  <si>
+    <t>b=4.2 mystery = 734_529.678</t>
+  </si>
+  <si>
+    <t>print(5+8j)</t>
+  </si>
+  <si>
+    <t>a=5</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>msg="Hello ", text='Hello '</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>my_list=[1,2,3,5]</t>
+  </si>
+  <si>
+    <t>create list</t>
+  </si>
+  <si>
+    <t>tuple(range(10))</t>
+  </si>
+  <si>
+    <t>create tuple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range(start,stop,step) -used to generate range of numbers from start to stop with step but not including stop number </t>
+  </si>
+  <si>
+    <t>isRain = True, isSun=False</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/</t>
+  </si>
+  <si>
+    <t>https://www.uifaces.co/</t>
+  </si>
+  <si>
+    <t>Avatars for design mockups</t>
+  </si>
+  <si>
+    <t>https://maketintsandshades.com/</t>
+  </si>
+  <si>
+    <t>Tint and shade generator</t>
+  </si>
+  <si>
+    <t>The internet’s source for visuals</t>
+  </si>
+  <si>
+    <t>https://ascii.co.uk/</t>
+  </si>
+  <si>
+    <t>The place for all things textual</t>
+  </si>
+  <si>
+    <t>https://devdocs.io/</t>
+  </si>
+  <si>
+    <t>Web development</t>
+  </si>
+  <si>
+    <t>Multiple API documentations in a fast, organized, and searchable interface</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org</t>
+  </si>
+  <si>
+    <t>HTML,CSS,Javascript</t>
+  </si>
+  <si>
+    <t>Online Python editor</t>
+  </si>
+  <si>
+    <t>https://replit.com</t>
+  </si>
+  <si>
+    <t>https://app.diagrams.net/</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t>Are in Capslock, for example</t>
+  </si>
+  <si>
+    <t>PI=3.141569</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -740,6 +824,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -795,10 +894,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -814,8 +914,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1128,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1256,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="14"/>
       <c r="D1" s="11" t="s">
@@ -1154,115 +1264,172 @@
       </c>
       <c r="E1" s="12"/>
       <c r="F1" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="14"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>201</v>
+      <c r="F2" s="15" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>202</v>
+      <c r="F3" s="15" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>203</v>
+      <c r="F4" s="15" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E5" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>9</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>199</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="D6" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="D7" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1287,285 +1454,285 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1579,7 +1746,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,239 +1760,239 @@
         <v>8</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1849,61 +2016,61 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="12"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1933,49 +2100,49 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -1983,21 +2150,21 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -2005,13 +2172,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2019,59 +2186,59 @@
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2085,26 +2252,27 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="67.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>188</v>
-      </c>
+      <c r="A1" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
+      <c r="A2" s="21" t="s">
+        <v>228</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2148,45 +2316,70 @@
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>187</v>
-      </c>
+      <c r="A15" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" s="12"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>189</v>
+      <c r="A16" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -2197,6 +2390,16 @@
       <c r="B23" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{5D22203B-BD37-4F7B-9EAC-7DF982024550}"/>
+    <hyperlink ref="A13" r:id="rId2" xr:uid="{1EDAC929-49B2-4450-AA63-98E4CB59A076}"/>
+    <hyperlink ref="A16" r:id="rId3" xr:uid="{982AA871-68B4-4D61-89AD-0A5169CDFE57}"/>
+    <hyperlink ref="A17" r:id="rId4" xr:uid="{9D2D357A-6808-4D9F-8448-CF155C325435}"/>
+    <hyperlink ref="A18" r:id="rId5" xr:uid="{F58A1396-A587-4866-998B-3F92275DCCF4}"/>
+    <hyperlink ref="A19" r:id="rId6" xr:uid="{F91E5413-1F5B-4940-AB32-19AEE9E8E0F6}"/>
+    <hyperlink ref="A20" r:id="rId7" xr:uid="{0130752C-BDB8-4B1F-BD9F-131689DE3F7A}"/>
+    <hyperlink ref="A2" r:id="rId8" xr:uid="{439D3B3C-D5B1-4755-A90C-E7CA8E4B6C1E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Python cheat sheet version 1.3 by Acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acopt\Desktop\My-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7DD949-5CA5-45A4-996A-C2BE6F8A19A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA2EF9A-DB6A-4489-93D4-84C36D6478AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="276">
   <si>
     <t>Data Conversion</t>
   </si>
@@ -279,9 +279,6 @@
   </si>
   <si>
     <t>number from 0 to 99, not including 100</t>
-  </si>
-  <si>
-    <t>Python Basics Cheat Sheet</t>
   </si>
   <si>
     <t>Learn Python with Acoptex: https://acoptex.lt</t>
@@ -666,9 +663,6 @@
     <t>for i in range(1,11,2): # not including 11</t>
   </si>
   <si>
-    <t>"one, two, three".split(", ")</t>
-  </si>
-  <si>
     <t>if "a" not in text:</t>
   </si>
   <si>
@@ -696,9 +690,6 @@
     <t>print(element) - prints the element to console</t>
   </si>
   <si>
-    <t>type(element)-returns the type of element</t>
-  </si>
-  <si>
     <t>b=4.2 mystery = 734_529.678</t>
   </si>
   <si>
@@ -720,15 +711,9 @@
     <t>my_list=[1,2,3,5]</t>
   </si>
   <si>
-    <t>create list</t>
-  </si>
-  <si>
     <t>tuple(range(10))</t>
   </si>
   <si>
-    <t>create tuple</t>
-  </si>
-  <si>
     <t xml:space="preserve">range(start,stop,step) -used to generate range of numbers from start to stop with step but not including stop number </t>
   </si>
   <si>
@@ -793,6 +778,205 @@
   </si>
   <si>
     <t>PI=3.141569</t>
+  </si>
+  <si>
+    <t>\'</t>
+  </si>
+  <si>
+    <t>Single Quote</t>
+  </si>
+  <si>
+    <t>\\</t>
+  </si>
+  <si>
+    <t>Backslash</t>
+  </si>
+  <si>
+    <t>\n</t>
+  </si>
+  <si>
+    <t>New Line</t>
+  </si>
+  <si>
+    <t>\r</t>
+  </si>
+  <si>
+    <t>Carriage Return</t>
+  </si>
+  <si>
+    <t>\t</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>\b</t>
+  </si>
+  <si>
+    <t>Backspace</t>
+  </si>
+  <si>
+    <t>\f</t>
+  </si>
+  <si>
+    <t>Form Feed</t>
+  </si>
+  <si>
+    <t>\ooo</t>
+  </si>
+  <si>
+    <t>Octal value</t>
+  </si>
+  <si>
+    <t>\xhh</t>
+  </si>
+  <si>
+    <t>Hex value</t>
+  </si>
+  <si>
+    <t>Escape Characters</t>
+  </si>
+  <si>
+    <t>Statement vs Expression</t>
+  </si>
+  <si>
+    <t>a = 100 -&gt; statement</t>
+  </si>
+  <si>
+    <t>b= a/2-&gt;statement</t>
+  </si>
+  <si>
+    <t>a/2 -&gt; expression</t>
+  </si>
+  <si>
+    <t>Operator precedence PEMDAS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. parenthesis </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(a+b)*c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. exponentiation </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a**b</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. multiplication / division </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a*b and a/b</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. addition / subtraction </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a+b and a-b</t>
+    </r>
+  </si>
+  <si>
+    <t>Python Basics Cheat Sheet version 1.3</t>
+  </si>
+  <si>
+    <t>\"</t>
+  </si>
+  <si>
+    <t>Double Quotes</t>
+  </si>
+  <si>
+    <t>type(element)-returns the class(data type) of element</t>
+  </si>
+  <si>
+    <t>bool("True")</t>
+  </si>
+  <si>
+    <t>list((1,2,3))</t>
+  </si>
+  <si>
+    <t>dict()</t>
+  </si>
+  <si>
+    <t>list-&gt;set</t>
+  </si>
+  <si>
+    <t>set([1,2,3])</t>
+  </si>
+  <si>
+    <t>set-&gt;list</t>
+  </si>
+  <si>
+    <t>list({1,2,3})</t>
+  </si>
+  <si>
+    <t>"a b c d e".split(" ")</t>
+  </si>
+  <si>
+    <t>string-&gt;bool</t>
+  </si>
+  <si>
+    <t>range-&gt;list</t>
+  </si>
+  <si>
+    <t>tuple-&gt;list</t>
+  </si>
+  <si>
+    <t>list-&gt;string</t>
+  </si>
+  <si>
+    <t>",".join(["a","b"])</t>
+  </si>
+  <si>
+    <t>range-&gt;tuple</t>
+  </si>
+  <si>
+    <t>create dictionary</t>
+  </si>
+  <si>
+    <t>dict</t>
+  </si>
+  <si>
+    <t>d={key:value}</t>
   </si>
 </sst>
 </file>
@@ -1238,48 +1422,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="1.28515625" customWidth="1"/>
+    <col min="3" max="3" width="0.7109375" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="1" customWidth="1"/>
     <col min="6" max="6" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>83</v>
+        <v>255</v>
       </c>
       <c r="B1" s="14"/>
       <c r="D1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="12"/>
+        <v>246</v>
+      </c>
       <c r="F1" s="11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="14"/>
-      <c r="D2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>1</v>
+      <c r="D2" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1287,50 +1467,38 @@
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>4</v>
+        <v>224</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>5</v>
+        <v>225</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>199</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1338,98 +1506,301 @@
         <v>10</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="D6" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>209</v>
-      </c>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="D7" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>207</v>
-      </c>
+    <row r="7" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="A8" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="D8" s="11" t="s">
         <v>13</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>163</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>164</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>204</v>
+        <v>193</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>16</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>211</v>
+        <v>200</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>17</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="F31" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1454,285 +1825,285 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1746,7 +2117,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1901,10 +2272,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2067,10 +2438,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2100,49 +2471,49 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -2150,21 +2521,21 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -2172,13 +2543,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2186,59 +2557,59 @@
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2263,16 +2634,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2317,10 +2688,10 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2329,56 +2700,56 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B15" s="12"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cheat sheet version 1.4 by acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acopt\Desktop\My-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA2EF9A-DB6A-4489-93D4-84C36D6478AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A223AC03-0F7D-4CD9-B99C-F2248ABBFD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Various" sheetId="1" r:id="rId1"/>
-    <sheet name="Data-structures" sheetId="5" r:id="rId2"/>
-    <sheet name="Strings" sheetId="3" r:id="rId3"/>
+    <sheet name="Strings" sheetId="3" r:id="rId2"/>
+    <sheet name="Data-structures" sheetId="5" r:id="rId3"/>
     <sheet name="Modules" sheetId="4" r:id="rId4"/>
     <sheet name="Loops Conditions Ternary operat" sheetId="6" r:id="rId5"/>
     <sheet name="Links" sheetId="2" r:id="rId6"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="276">
-  <si>
-    <t>Data Conversion</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="305">
   <si>
     <t>string-&gt;int</t>
   </si>
@@ -71,9 +68,6 @@
     <t>else:</t>
   </si>
   <si>
-    <t>Operators</t>
-  </si>
-  <si>
     <t>and</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>for i in list:</t>
   </si>
   <si>
-    <t>immutable</t>
-  </si>
-  <si>
     <t>can be any of these strings</t>
   </si>
   <si>
@@ -119,9 +110,6 @@
     <t>text.find("a")</t>
   </si>
   <si>
-    <t>to find first a, if not find returns -1</t>
-  </si>
-  <si>
     <t>text.replace("o","a")</t>
   </si>
   <si>
@@ -173,9 +161,6 @@
     <t>text[start:stop:stepover]</t>
   </si>
   <si>
-    <t>string slicing</t>
-  </si>
-  <si>
     <t>text[index]</t>
   </si>
   <si>
@@ -287,9 +272,6 @@
     <t>nums=[1,2,3,4,5]</t>
   </si>
   <si>
-    <t>nums[::-1] reverse of list</t>
-  </si>
-  <si>
     <t>len(nums)</t>
   </si>
   <si>
@@ -401,18 +383,6 @@
     <t>list(range(10))</t>
   </si>
   <si>
-    <t>create a list</t>
-  </si>
-  <si>
-    <t>list((1,2,3,4))</t>
-  </si>
-  <si>
-    <t>create a list from tuple</t>
-  </si>
-  <si>
-    <t>[(1,2),2] or ([1,2],2)</t>
-  </si>
-  <si>
     <t>can nest tuples in lists and lists in tuples</t>
   </si>
   <si>
@@ -471,15 +441,6 @@
   </si>
   <si>
     <t>reverse the elements in the list</t>
-  </si>
-  <si>
-    <t>list to string</t>
-  </si>
-  <si>
-    <t>".".join(nums)</t>
-  </si>
-  <si>
-    <t>mutable, mixed data types</t>
   </si>
   <si>
     <t>num[0]=0</t>
@@ -672,15 +633,6 @@
     <t>Data types</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>complex</t>
-  </si>
-  <si>
     <t>Functions</t>
   </si>
   <si>
@@ -696,18 +648,9 @@
     <t>print(5+8j)</t>
   </si>
   <si>
-    <t>a=5</t>
-  </si>
-  <si>
-    <t>str</t>
-  </si>
-  <si>
     <t>msg="Hello ", text='Hello '</t>
   </si>
   <si>
-    <t>list</t>
-  </si>
-  <si>
     <t>my_list=[1,2,3,5]</t>
   </si>
   <si>
@@ -718,9 +661,6 @@
   </si>
   <si>
     <t>isRain = True, isSun=False</t>
-  </si>
-  <si>
-    <t>bool</t>
   </si>
   <si>
     <t>https://unsplash.com/</t>
@@ -916,9 +856,6 @@
     </r>
   </si>
   <si>
-    <t>Python Basics Cheat Sheet version 1.3</t>
-  </si>
-  <si>
     <t>\"</t>
   </si>
   <si>
@@ -928,9 +865,6 @@
     <t>type(element)-returns the class(data type) of element</t>
   </si>
   <si>
-    <t>bool("True")</t>
-  </si>
-  <si>
     <t>list((1,2,3))</t>
   </si>
   <si>
@@ -973,10 +907,175 @@
     <t>create dictionary</t>
   </si>
   <si>
-    <t>dict</t>
-  </si>
-  <si>
     <t>d={key:value}</t>
+  </si>
+  <si>
+    <t>a=2, Large numbers: 125_456_456</t>
+  </si>
+  <si>
+    <t>fruits_in_room=None</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>a,b=1,2</t>
+  </si>
+  <si>
+    <t>x=1</t>
+  </si>
+  <si>
+    <t>a,b=b,a</t>
+  </si>
+  <si>
+    <t>x=1;b=2</t>
+  </si>
+  <si>
+    <t>Variable Assignment</t>
+  </si>
+  <si>
+    <t>string slicing, stop not included</t>
+  </si>
+  <si>
+    <t>reverse the order of string</t>
+  </si>
+  <si>
+    <t>text="0123456" text[::-1]</t>
+  </si>
+  <si>
+    <t>https://docs.python.org/3/library/functions.html</t>
+  </si>
+  <si>
+    <t>Built-in Functions</t>
+  </si>
+  <si>
+    <t>text.capitalize()</t>
+  </si>
+  <si>
+    <t>converts the first character of the string to a capital letter, while making all other characters in the string lowercase letters.</t>
+  </si>
+  <si>
+    <t>to find index of first letter a, if not find returns -1</t>
+  </si>
+  <si>
+    <t>bool("True"),bool(0),bool(1)</t>
+  </si>
+  <si>
+    <t>float (floating point number)</t>
+  </si>
+  <si>
+    <t>complex (complex number)</t>
+  </si>
+  <si>
+    <t>int (integer number)</t>
+  </si>
+  <si>
+    <t>str (string)</t>
+  </si>
+  <si>
+    <t>bool (boolean)</t>
+  </si>
+  <si>
+    <t>list (list)</t>
+  </si>
+  <si>
+    <t>dict (dictionary)</t>
+  </si>
+  <si>
+    <t>Data type conversion</t>
+  </si>
+  <si>
+    <t>https://realpython.com/python-comments-guide/</t>
+  </si>
+  <si>
+    <t>Comments guide</t>
+  </si>
+  <si>
+    <t>mutable, mixed data types, ordered</t>
+  </si>
+  <si>
+    <t>immutable, ordered</t>
+  </si>
+  <si>
+    <t>division -&gt;integer</t>
+  </si>
+  <si>
+    <t>a//b</t>
+  </si>
+  <si>
+    <t>division -&gt;float</t>
+  </si>
+  <si>
+    <t>a/b</t>
+  </si>
+  <si>
+    <t>remainder</t>
+  </si>
+  <si>
+    <t>a%b</t>
+  </si>
+  <si>
+    <t>exponentiation</t>
+  </si>
+  <si>
+    <t>a**b</t>
+  </si>
+  <si>
+    <t>multiplication</t>
+  </si>
+  <si>
+    <t>a*b</t>
+  </si>
+  <si>
+    <t>subtraction</t>
+  </si>
+  <si>
+    <t>a-b</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>a+b</t>
+  </si>
+  <si>
+    <t>Arithmetic operators</t>
+  </si>
+  <si>
+    <t>Boolean operators</t>
+  </si>
+  <si>
+    <t>example of list</t>
+  </si>
+  <si>
+    <t>Unpacking</t>
+  </si>
+  <si>
+    <t>Works with lists, tuples</t>
+  </si>
+  <si>
+    <t>new_list=list[:]</t>
+  </si>
+  <si>
+    <t>Copy the whole list to new_list</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[(1,2),2] or ([1,2],2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (matrix)</t>
+    </r>
+  </si>
+  <si>
+    <t>Python Basics Cheat Sheet version 1.4</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1099,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1008,6 +1106,7 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1082,18 +1181,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
@@ -1103,10 +1197,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1422,385 +1520,483 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F43"/>
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="0.7109375" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" customWidth="1"/>
     <col min="5" max="5" width="1" customWidth="1"/>
     <col min="6" max="6" width="46.7109375" customWidth="1"/>
+    <col min="7" max="7" width="0.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="14"/>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="D1" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="9"/>
       <c r="D2" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>224</v>
+        <v>227</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>204</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="F4" s="15" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="F8" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="D8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>192</v>
+        <v>270</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>181</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
     <row r="18" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="B19" s="12"/>
+      <c r="A19" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="F31" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="F31" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="F32" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="B33" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="15" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>273</v>
+        <v>239</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="D45" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -1810,314 +2006,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67167C2-0A1D-4D6A-8A81-1046F3A6BE4C}">
-  <dimension ref="A1:B36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F34158-7427-4D01-A333-AC1EF8F5E41A}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F34158-7427-4D01-A333-AC1EF8F5E41A}">
-  <dimension ref="A1:B30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,243 +2023,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B7" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="B20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="B22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="B23" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="B27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="B28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="B29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="B30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="1" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="B31" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>67</v>
+      <c r="B32" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2371,8 +2283,329 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67167C2-0A1D-4D6A-8A81-1046F3A6BE4C}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:M35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.85546875" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="1.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B2042D-D8FE-438B-8520-CFD02283ED1B}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2387,61 +2620,61 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="12"/>
+      <c r="A2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2452,6 +2685,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6D0CCE-B929-4986-83C2-2FA089974AB9}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2471,145 +2707,145 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>179</v>
+        <v>142</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>179</v>
+      <c r="A16" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2620,156 +2856,154 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4C525F-6578-4FBF-AF5B-25D694809E3A}">
-  <dimension ref="A1:B23"/>
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="2" width="67.140625" customWidth="1"/>
+    <col min="3" max="3" width="1.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="12"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="D1" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="B13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="B15" s="12"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1" xr:uid="{5D22203B-BD37-4F7B-9EAC-7DF982024550}"/>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{5D22203B-BD37-4F7B-9EAC-7DF982024550}"/>
     <hyperlink ref="A13" r:id="rId2" xr:uid="{1EDAC929-49B2-4450-AA63-98E4CB59A076}"/>
-    <hyperlink ref="A16" r:id="rId3" xr:uid="{982AA871-68B4-4D61-89AD-0A5169CDFE57}"/>
-    <hyperlink ref="A17" r:id="rId4" xr:uid="{9D2D357A-6808-4D9F-8448-CF155C325435}"/>
-    <hyperlink ref="A18" r:id="rId5" xr:uid="{F58A1396-A587-4866-998B-3F92275DCCF4}"/>
-    <hyperlink ref="A19" r:id="rId6" xr:uid="{F91E5413-1F5B-4940-AB32-19AEE9E8E0F6}"/>
-    <hyperlink ref="A20" r:id="rId7" xr:uid="{0130752C-BDB8-4B1F-BD9F-131689DE3F7A}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{982AA871-68B4-4D61-89AD-0A5169CDFE57}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{9D2D357A-6808-4D9F-8448-CF155C325435}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{F58A1396-A587-4866-998B-3F92275DCCF4}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{F91E5413-1F5B-4940-AB32-19AEE9E8E0F6}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{0130752C-BDB8-4B1F-BD9F-131689DE3F7A}"/>
     <hyperlink ref="A2" r:id="rId8" xr:uid="{439D3B3C-D5B1-4755-A90C-E7CA8E4B6C1E}"/>
+    <hyperlink ref="A3" r:id="rId9" xr:uid="{DDDF39EE-66EA-4D37-9C3D-7692538D5B17}"/>
+    <hyperlink ref="A4" r:id="rId10" xr:uid="{E0A2B512-EFAE-483F-AE74-5BDC7C552F7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cheat sheet version 1.5 by acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acopt\Desktop\My-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A223AC03-0F7D-4CD9-B99C-F2248ABBFD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B68E9C2-AE9A-4040-B0BF-1A1B63577340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="362">
   <si>
     <t>string-&gt;int</t>
   </si>
@@ -393,9 +393,6 @@
   </si>
   <si>
     <t>sorted(nums)</t>
-  </si>
-  <si>
-    <t>produce new list sorted</t>
   </si>
   <si>
     <t>my_list=[[1,2,3],[4,5,6],[7,8,9]]</t>
@@ -907,9 +904,6 @@
     <t>create dictionary</t>
   </si>
   <si>
-    <t>d={key:value}</t>
-  </si>
-  <si>
     <t>a=2, Large numbers: 125_456_456</t>
   </si>
   <si>
@@ -974,9 +968,6 @@
   </si>
   <si>
     <t>bool (boolean)</t>
-  </si>
-  <si>
-    <t>list (list)</t>
   </si>
   <si>
     <t>dict (dictionary)</t>
@@ -1075,7 +1066,187 @@
     </r>
   </si>
   <si>
-    <t>Python Basics Cheat Sheet version 1.4</t>
+    <t>my_tuple=(1,2,4,9)</t>
+  </si>
+  <si>
+    <t>tuple</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>my_dict={"Alex":145}</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>my_set={'Alex','Olga'}</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>class MyClass:</t>
+  </si>
+  <si>
+    <t>OOP</t>
+  </si>
+  <si>
+    <t>Dictionaries</t>
+  </si>
+  <si>
+    <t>my_dict={"Alex":(1,2,3)}</t>
+  </si>
+  <si>
+    <t>can contain tuples, lists, sets, dictionaries</t>
+  </si>
+  <si>
+    <t>len(user1)</t>
+  </si>
+  <si>
+    <t>length of dictionary</t>
+  </si>
+  <si>
+    <t>user1[key]</t>
+  </si>
+  <si>
+    <t>get the value by key</t>
+  </si>
+  <si>
+    <t>user1[key1]=value1</t>
+  </si>
+  <si>
+    <t>user1.get(key1)</t>
+  </si>
+  <si>
+    <t>user1.get(key1, 55)</t>
+  </si>
+  <si>
+    <t>if no key1, then value 55</t>
+  </si>
+  <si>
+    <t>user1={}</t>
+  </si>
+  <si>
+    <t>clears the elements of dictionary</t>
+  </si>
+  <si>
+    <t>user1.update({key1: value1})</t>
+  </si>
+  <si>
+    <t>add key and value pair to dict</t>
+  </si>
+  <si>
+    <t>user1.update({key1: value2})</t>
+  </si>
+  <si>
+    <t>can also update value if key exist</t>
+  </si>
+  <si>
+    <t>del user1[key]</t>
+  </si>
+  <si>
+    <t>delete element from dictionary</t>
+  </si>
+  <si>
+    <t>user1.keys()</t>
+  </si>
+  <si>
+    <t>list of all keys in dictionary</t>
+  </si>
+  <si>
+    <t>user1.values()</t>
+  </si>
+  <si>
+    <t>list of all values in dictionary</t>
+  </si>
+  <si>
+    <t>user1.items()</t>
+  </si>
+  <si>
+    <t>list of key and value pairs</t>
+  </si>
+  <si>
+    <t>user1.pop(key1)</t>
+  </si>
+  <si>
+    <t>removes key and value from dictionary</t>
+  </si>
+  <si>
+    <t>if "" in user1:</t>
+  </si>
+  <si>
+    <t>if element included in dictionary True/False</t>
+  </si>
+  <si>
+    <t>user1.clear()</t>
+  </si>
+  <si>
+    <t>for key in user1:</t>
+  </si>
+  <si>
+    <t>iterate through dictionary</t>
+  </si>
+  <si>
+    <t>print(key)</t>
+  </si>
+  <si>
+    <t>and get values</t>
+  </si>
+  <si>
+    <t>print(user1[key])</t>
+  </si>
+  <si>
+    <t>if 'key1' in / not in user1:</t>
+  </si>
+  <si>
+    <t>if key in or not in dictionary</t>
+  </si>
+  <si>
+    <t>my_dict["Alex"][1]-&gt;2</t>
+  </si>
+  <si>
+    <t>dictionary slicing</t>
+  </si>
+  <si>
+    <t>user2=dict(name="Alex")</t>
+  </si>
+  <si>
+    <t>created user with name Alex</t>
+  </si>
+  <si>
+    <t>user1.copy()</t>
+  </si>
+  <si>
+    <t>returns a copy of dictionary</t>
+  </si>
+  <si>
+    <t>user1.popitem()</t>
+  </si>
+  <si>
+    <t>random removal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user1={key:value,key2:value2} </t>
+  </si>
+  <si>
+    <t>example of dictionaries/ doesn't account dublicates</t>
+  </si>
+  <si>
+    <t>check for key in dictionary -&gt;None</t>
+  </si>
+  <si>
+    <t>add new element to dictionary/edit the value of existing key</t>
+  </si>
+  <si>
+    <t>mutable, key can not be changed and must be unique</t>
+  </si>
+  <si>
+    <t>produce new sorted list</t>
+  </si>
+  <si>
+    <t>Python Basics Cheat Sheet version 1.5</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1192,19 +1363,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1523,10 +1689,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,18 +1705,19 @@
     <col min="6" max="6" width="46.7109375" customWidth="1"/>
     <col min="7" max="7" width="0.7109375" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>304</v>
+        <v>361</v>
       </c>
       <c r="B1" s="9"/>
       <c r="D1" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1559,10 +1726,10 @@
       </c>
       <c r="B2" s="9"/>
       <c r="D2" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>179</v>
+        <v>226</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1570,41 +1737,41 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>180</v>
+        <v>227</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>237</v>
+        <v>228</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>186</v>
+        <v>296</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1613,390 +1780,409 @@
       </c>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="11"/>
-    </row>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B8" s="7"/>
       <c r="F8" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>233</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>183</v>
+        <v>271</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>275</v>
+        <v>303</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>252</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>255</v>
+        <v>305</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="B19" s="7"/>
-    </row>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>208</v>
-      </c>
+      <c r="A20" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>209</v>
+        <v>234</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="F31" s="1" t="s">
+    </row>
+    <row r="31" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="F32" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B34" s="10" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B37" s="10" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B42" s="10" t="s">
+      <c r="B44" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="B45" s="6"/>
-      <c r="D45" s="6" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B46" s="1" t="s">
+    <row r="45" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="D46" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="D46" s="1" t="s">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D47" s="1" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2027,11 +2213,11 @@
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2039,7 +2225,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2047,7 +2233,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2055,15 +2241,15 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>266</v>
+      <c r="A5" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2071,15 +2257,15 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2087,7 +2273,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2095,7 +2281,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2103,7 +2289,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2111,7 +2297,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2119,7 +2305,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2127,7 +2313,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2135,7 +2321,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2143,23 +2329,23 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>263</v>
-      </c>
       <c r="B17" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2167,7 +2353,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2175,7 +2361,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2183,15 +2369,15 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2199,7 +2385,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2207,7 +2393,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2215,7 +2401,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2223,7 +2409,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2231,7 +2417,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2239,7 +2425,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2247,7 +2433,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2255,7 +2441,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2263,7 +2449,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2271,7 +2457,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2290,8 +2476,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2299,11 +2485,13 @@
     <col min="1" max="1" width="38.85546875" customWidth="1"/>
     <col min="2" max="2" width="45.5703125" customWidth="1"/>
     <col min="3" max="3" width="1.28515625" customWidth="1"/>
+    <col min="4" max="4" width="53.42578125" customWidth="1"/>
+    <col min="5" max="5" width="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -2319,120 +2507,186 @@
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>133</v>
+      <c r="D5" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>138</v>
+      <c r="D6" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="D7" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="1"/>
+      <c r="D8" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="D9" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="D10" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="D11" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="D12" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="D13" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="D14" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>134</v>
+      <c r="A15" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2442,157 +2696,233 @@
       <c r="B16" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="D16" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>301</v>
+      <c r="D17" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="D19" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="D21" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="D22" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="D23" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="D24" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="D25" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="D26" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>303</v>
+      <c r="D27" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="D28" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="B31" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="B32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="1" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="B33" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B33" s="1" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="B34" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B34" s="1" t="s">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="B35" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2671,10 +3001,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2707,49 +3037,49 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -2757,21 +3087,21 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -2779,13 +3109,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2793,59 +3123,59 @@
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2876,84 +3206,84 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" s="7"/>
       <c r="D1" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>198</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="A3" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>195</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>279</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>193</v>
+      <c r="A4" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>189</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>191</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>199</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2981,11 +3311,11 @@
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B13" s="16" t="s">
+      <c r="A13" s="11" t="s">
         <v>201</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cheat sheet version 1.6 by acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acopt\Desktop\My-Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\2-Python-cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B68E9C2-AE9A-4040-B0BF-1A1B63577340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14F9927-A093-4E1C-9776-38200ACDCDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Various" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Data-structures" sheetId="5" r:id="rId3"/>
     <sheet name="Modules" sheetId="4" r:id="rId4"/>
     <sheet name="Loops Conditions Ternary operat" sheetId="6" r:id="rId5"/>
-    <sheet name="Links" sheetId="2" r:id="rId6"/>
+    <sheet name="Command prompt Terminal command" sheetId="7" r:id="rId6"/>
+    <sheet name="Links" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="462">
   <si>
     <t>string-&gt;int</t>
   </si>
@@ -66,18 +67,6 @@
   </si>
   <si>
     <t>else:</t>
-  </si>
-  <si>
-    <t>and</t>
-  </si>
-  <si>
-    <t>or</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>not</t>
   </si>
   <si>
     <t>elif condition:</t>
@@ -865,9 +854,6 @@
     <t>list((1,2,3))</t>
   </si>
   <si>
-    <t>dict()</t>
-  </si>
-  <si>
     <t>list-&gt;set</t>
   </si>
   <si>
@@ -1031,9 +1017,6 @@
   </si>
   <si>
     <t>Arithmetic operators</t>
-  </si>
-  <si>
-    <t>Boolean operators</t>
   </si>
   <si>
     <t>example of list</t>
@@ -1108,102 +1091,30 @@
     <t>length of dictionary</t>
   </si>
   <si>
-    <t>user1[key]</t>
-  </si>
-  <si>
     <t>get the value by key</t>
   </si>
   <si>
-    <t>user1[key1]=value1</t>
-  </si>
-  <si>
-    <t>user1.get(key1)</t>
-  </si>
-  <si>
-    <t>user1.get(key1, 55)</t>
-  </si>
-  <si>
-    <t>if no key1, then value 55</t>
-  </si>
-  <si>
-    <t>user1={}</t>
-  </si>
-  <si>
     <t>clears the elements of dictionary</t>
   </si>
   <si>
-    <t>user1.update({key1: value1})</t>
-  </si>
-  <si>
-    <t>add key and value pair to dict</t>
-  </si>
-  <si>
-    <t>user1.update({key1: value2})</t>
-  </si>
-  <si>
     <t>can also update value if key exist</t>
   </si>
   <si>
-    <t>del user1[key]</t>
-  </si>
-  <si>
     <t>delete element from dictionary</t>
   </si>
   <si>
-    <t>user1.keys()</t>
-  </si>
-  <si>
     <t>list of all keys in dictionary</t>
   </si>
   <si>
-    <t>user1.values()</t>
-  </si>
-  <si>
     <t>list of all values in dictionary</t>
   </si>
   <si>
-    <t>user1.items()</t>
-  </si>
-  <si>
     <t>list of key and value pairs</t>
   </si>
   <si>
-    <t>user1.pop(key1)</t>
-  </si>
-  <si>
-    <t>removes key and value from dictionary</t>
-  </si>
-  <si>
-    <t>if "" in user1:</t>
-  </si>
-  <si>
-    <t>if element included in dictionary True/False</t>
-  </si>
-  <si>
-    <t>user1.clear()</t>
-  </si>
-  <si>
-    <t>for key in user1:</t>
-  </si>
-  <si>
     <t>iterate through dictionary</t>
   </si>
   <si>
-    <t>print(key)</t>
-  </si>
-  <si>
-    <t>and get values</t>
-  </si>
-  <si>
-    <t>print(user1[key])</t>
-  </si>
-  <si>
-    <t>if 'key1' in / not in user1:</t>
-  </si>
-  <si>
-    <t>if key in or not in dictionary</t>
-  </si>
-  <si>
     <t>my_dict["Alex"][1]-&gt;2</t>
   </si>
   <si>
@@ -1216,21 +1127,9 @@
     <t>created user with name Alex</t>
   </si>
   <si>
-    <t>user1.copy()</t>
-  </si>
-  <si>
     <t>returns a copy of dictionary</t>
   </si>
   <si>
-    <t>user1.popitem()</t>
-  </si>
-  <si>
-    <t>random removal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user1={key:value,key2:value2} </t>
-  </si>
-  <si>
     <t>example of dictionaries/ doesn't account dublicates</t>
   </si>
   <si>
@@ -1246,7 +1145,409 @@
     <t>produce new sorted list</t>
   </si>
   <si>
-    <t>Python Basics Cheat Sheet version 1.5</t>
+    <t>a,b,c=[1,2,3]</t>
+  </si>
+  <si>
+    <t>How to import modules</t>
+  </si>
+  <si>
+    <t>from random import randint</t>
+  </si>
+  <si>
+    <t>The whole module imported</t>
+  </si>
+  <si>
+    <t>Imported randint function only</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>http://getskeleton.com/</t>
+  </si>
+  <si>
+    <t>A dead simple, responsive boilerplate.</t>
+  </si>
+  <si>
+    <t>Python Basics Cheat Sheet version 1.6</t>
+  </si>
+  <si>
+    <t>a,b=(1,2)</t>
+  </si>
+  <si>
+    <t>a+=1 b-=2 c*=3 b/=4</t>
+  </si>
+  <si>
+    <t>Augmented assignment operators</t>
+  </si>
+  <si>
+    <t>a==b a!=b a&lt;b b&gt;c d&lt;=e f&gt;=t</t>
+  </si>
+  <si>
+    <t>Comparison operators</t>
+  </si>
+  <si>
+    <t>and or not</t>
+  </si>
+  <si>
+    <t>Logical operators</t>
+  </si>
+  <si>
+    <t>my_list=[{key:value},[1,2,3],[4,5,6],[7,8,9]]</t>
+  </si>
+  <si>
+    <t>can contain dictionaries too</t>
+  </si>
+  <si>
+    <t>dict(name="Alex")</t>
+  </si>
+  <si>
+    <t>for i in dict:</t>
+  </si>
+  <si>
+    <t>for i in tuple:</t>
+  </si>
+  <si>
+    <t>Command prompt</t>
+  </si>
+  <si>
+    <t>Terminal</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>present working directory</t>
+  </si>
+  <si>
+    <t>cd directory</t>
+  </si>
+  <si>
+    <t>change to directory</t>
+  </si>
+  <si>
+    <t>ls</t>
+  </si>
+  <si>
+    <t>cd ..</t>
+  </si>
+  <si>
+    <t>brings back to one directory back</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>clear the terminal</t>
+  </si>
+  <si>
+    <t>cd /</t>
+  </si>
+  <si>
+    <t>go to root directory</t>
+  </si>
+  <si>
+    <t>cd ~</t>
+  </si>
+  <si>
+    <t>go to user directory</t>
+  </si>
+  <si>
+    <t>open .</t>
+  </si>
+  <si>
+    <t>opens current folder</t>
+  </si>
+  <si>
+    <t>mkdir directory</t>
+  </si>
+  <si>
+    <t>touch index.html</t>
+  </si>
+  <si>
+    <t>open index.html</t>
+  </si>
+  <si>
+    <t>open file</t>
+  </si>
+  <si>
+    <t>open -a "Sublime text"</t>
+  </si>
+  <si>
+    <t>open sublime text</t>
+  </si>
+  <si>
+    <t>open -a "Sublime text" index.html</t>
+  </si>
+  <si>
+    <t>open sublime text index.html</t>
+  </si>
+  <si>
+    <t>mv index.html about.html</t>
+  </si>
+  <si>
+    <t>rename file</t>
+  </si>
+  <si>
+    <t>rm about.html</t>
+  </si>
+  <si>
+    <t>remove file</t>
+  </si>
+  <si>
+    <t>rm -r directory</t>
+  </si>
+  <si>
+    <t>remove folder</t>
+  </si>
+  <si>
+    <t>list all the files in current directory</t>
+  </si>
+  <si>
+    <t>dir</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>makes directory</t>
+  </si>
+  <si>
+    <t>creates file</t>
+  </si>
+  <si>
+    <t>https://peps.python.org/pep-0008/</t>
+  </si>
+  <si>
+    <t>PEP 8 – Style Guide for Python Code</t>
+  </si>
+  <si>
+    <t>https://www.postgresql.org/download/</t>
+  </si>
+  <si>
+    <t>https://www.enterprisedb.com/downloads/postgres-postgresql-downloads</t>
+  </si>
+  <si>
+    <t>Database for Django all Oses</t>
+  </si>
+  <si>
+    <t>Database for Django for Windows</t>
+  </si>
+  <si>
+    <t>https://www.pgadmin.org/download/</t>
+  </si>
+  <si>
+    <t>pgAdmin is the most popular and feature rich Open Source administration and development platform for PostgreSQL, the most advanced Open Source database in the world.</t>
+  </si>
+  <si>
+    <t>https://packagecontrol.io/</t>
+  </si>
+  <si>
+    <t>The Sublime Text package manager that makes it exceedingly simple to find, install and keep packages up-to-date.</t>
+  </si>
+  <si>
+    <t>python version check</t>
+  </si>
+  <si>
+    <t>python --version</t>
+  </si>
+  <si>
+    <t>Install Django</t>
+  </si>
+  <si>
+    <t>python -m pip install Django</t>
+  </si>
+  <si>
+    <t>django-admin</t>
+  </si>
+  <si>
+    <t>To verify Django tool installed</t>
+  </si>
+  <si>
+    <t>django-admin startproject mypage</t>
+  </si>
+  <si>
+    <t>New Django project</t>
+  </si>
+  <si>
+    <t>pip install flask</t>
+  </si>
+  <si>
+    <t>flask --version</t>
+  </si>
+  <si>
+    <t>Check for Flask version</t>
+  </si>
+  <si>
+    <t>Install Flask</t>
+  </si>
+  <si>
+    <t>opencv</t>
+  </si>
+  <si>
+    <t>openblas</t>
+  </si>
+  <si>
+    <t>Anaconda environment</t>
+  </si>
+  <si>
+    <t>https://www.qt.io/</t>
+  </si>
+  <si>
+    <t>QT</t>
+  </si>
+  <si>
+    <t>pyqt</t>
+  </si>
+  <si>
+    <t>qtpy</t>
+  </si>
+  <si>
+    <t>returns value, removes key and value from dictionary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dictionary={key:value,key2:value2} </t>
+  </si>
+  <si>
+    <t>dictionary[key]</t>
+  </si>
+  <si>
+    <t>dictionary[key1]=value1</t>
+  </si>
+  <si>
+    <t>dictionary.get(key1)</t>
+  </si>
+  <si>
+    <t>dictionary.get(key1, 55)</t>
+  </si>
+  <si>
+    <t>if no key1, then value will be 55</t>
+  </si>
+  <si>
+    <t>dictionary={}</t>
+  </si>
+  <si>
+    <t>dictionary.update({key1: value1})</t>
+  </si>
+  <si>
+    <t>dictionary.update({key1: value2})</t>
+  </si>
+  <si>
+    <t>removes last key/value pair</t>
+  </si>
+  <si>
+    <t>dictionary.copy()</t>
+  </si>
+  <si>
+    <t>if "key" in dictionary:</t>
+  </si>
+  <si>
+    <t>if key included in dictionary True/False</t>
+  </si>
+  <si>
+    <t>dictionary.clear()</t>
+  </si>
+  <si>
+    <t>dictionary.pop(key1)</t>
+  </si>
+  <si>
+    <t>del dictionary[key]</t>
+  </si>
+  <si>
+    <t>dictionary.keys()</t>
+  </si>
+  <si>
+    <t>dictionary.values()</t>
+  </si>
+  <si>
+    <t>dictionary.items()</t>
+  </si>
+  <si>
+    <t>for key in dictionary:</t>
+  </si>
+  <si>
+    <t>if "key" not in dictionary:</t>
+  </si>
+  <si>
+    <t>dictionary.popitem()</t>
+  </si>
+  <si>
+    <t>add key and value pair to dictionary</t>
+  </si>
+  <si>
+    <t>Tuples</t>
+  </si>
+  <si>
+    <t>immutable</t>
+  </si>
+  <si>
+    <t>text="test" if True else "ready"</t>
+  </si>
+  <si>
+    <t>my_tuple=(1,"Alex", "Rose", 5)</t>
+  </si>
+  <si>
+    <t>my_tuple[0]</t>
+  </si>
+  <si>
+    <t>tuple indexing</t>
+  </si>
+  <si>
+    <t>my_tuple.index(element)</t>
+  </si>
+  <si>
+    <t>returns index of element</t>
+  </si>
+  <si>
+    <t>my_tuple.count(element)</t>
+  </si>
+  <si>
+    <t>counts number of elements in tuple</t>
+  </si>
+  <si>
+    <t>[(1,2),2] or ([1,2],2)</t>
+  </si>
+  <si>
+    <t>x, y, z, *other= my_tuple</t>
+  </si>
+  <si>
+    <t>unpacking the tuple</t>
+  </si>
+  <si>
+    <t>my_tuple[start:stop:-1]</t>
+  </si>
+  <si>
+    <t>tuple slicing</t>
+  </si>
+  <si>
+    <t>for x in my_tuple:</t>
+  </si>
+  <si>
+    <t>use for loop to iterate through tuple</t>
+  </si>
+  <si>
+    <t>len(my_tuple)</t>
+  </si>
+  <si>
+    <t>number of elements in tuple</t>
+  </si>
+  <si>
+    <t>if 'a' in my_tuple:</t>
+  </si>
+  <si>
+    <t>if string a is in tuple True/False</t>
+  </si>
+  <si>
+    <t>my_tuple=((1,2),4)</t>
+  </si>
+  <si>
+    <t>can be nested tuples in tuples</t>
+  </si>
+  <si>
+    <t>example of tuple</t>
+  </si>
+  <si>
+    <t>a,b,c=(1,2,3)</t>
   </si>
 </sst>
 </file>
@@ -1352,10 +1653,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1370,7 +1670,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1692,7 +1995,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,78 +2003,76 @@
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="0.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="1" customWidth="1"/>
     <col min="6" max="6" width="46.7109375" customWidth="1"/>
     <col min="7" max="7" width="0.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="D1" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>177</v>
+      <c r="A1" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="F1" s="5" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="D2" s="1" t="s">
-        <v>226</v>
-      </c>
+      <c r="A2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="F2" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>227</v>
+      <c r="B3" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>221</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>172</v>
+      <c r="A4" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>296</v>
+        <v>201</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1780,232 +2081,250 @@
       </c>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>297</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="F8" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="I8" s="6"/>
+      <c r="A8" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="D8" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>461</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="I11" s="7"/>
+        <v>228</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>308</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>186</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="B20" s="7"/>
+      <c r="A20" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="B32" s="7"/>
+      <c r="A32" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B32" s="6"/>
       <c r="F32" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2016,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2029,15 +2348,15 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>8</v>
@@ -2053,136 +2372,139 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>184</v>
+      <c r="A43" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>238</v>
+        <v>345</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="B46" s="6"/>
-      <c r="D46" s="6" t="s">
-        <v>294</v>
+      <c r="A46" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="D46" s="5" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>12</v>
+        <v>286</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>13</v>
+        <v>284</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>14</v>
+        <v>282</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>15</v>
+        <v>280</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2199,7 +2521,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,259 +2531,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>278</v>
+      <c r="B1" s="5" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>55</v>
+      <c r="A27" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2474,10 +2796,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2487,442 +2809,512 @@
     <col min="3" max="3" width="1.28515625" customWidth="1"/>
     <col min="4" max="4" width="53.42578125" customWidth="1"/>
     <col min="5" max="5" width="48" customWidth="1"/>
+    <col min="6" max="6" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="D3" s="6" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="D15" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="15" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="E6" s="15" t="s">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="D21" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="15" t="s">
-        <v>317</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>323</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>325</v>
-      </c>
-      <c r="E13" s="15" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="E23" s="15" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="15" t="s">
+      <c r="B29" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>347</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="16" t="s">
+        <v>441</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" s="16" t="s">
+        <v>445</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D33" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>130</v>
+        <v>87</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>452</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="16" t="s">
+        <v>456</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -2936,76 +3328,122 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="1.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="7"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>140</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3018,10 +3456,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3036,72 +3474,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>166</v>
+      <c r="A1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -3109,73 +3547,95 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>165</v>
+        <v>137</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>163</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>145</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>146</v>
+        <v>347</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>165</v>
+      <c r="A16" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3185,14 +3645,242 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DBE735-7267-40D5-BEF9-3555817B665F}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A25:A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="1.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="D1" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4C525F-6578-4FBF-AF5B-25D694809E3A}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3205,122 +3893,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="D1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="D1" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="D6" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="D5" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="D6" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="D7" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>200</v>
-      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="D14" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>409</v>
+      </c>
+      <c r="B16" t="s">
+        <v>410</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3334,6 +4064,11 @@
     <hyperlink ref="A2" r:id="rId8" xr:uid="{439D3B3C-D5B1-4755-A90C-E7CA8E4B6C1E}"/>
     <hyperlink ref="A3" r:id="rId9" xr:uid="{DDDF39EE-66EA-4D37-9C3D-7692538D5B17}"/>
     <hyperlink ref="A4" r:id="rId10" xr:uid="{E0A2B512-EFAE-483F-AE74-5BDC7C552F7E}"/>
+    <hyperlink ref="D8" r:id="rId11" xr:uid="{7B3684F7-A2D7-482D-94C2-C1EEBDC8CE68}"/>
+    <hyperlink ref="A5" r:id="rId12" xr:uid="{BE87A156-080B-4A7E-A532-4232974EBB0F}"/>
+    <hyperlink ref="A8" r:id="rId13" xr:uid="{23507FA9-2015-4A48-9B33-9831ED449069}"/>
+    <hyperlink ref="A7" r:id="rId14" xr:uid="{65E1EF1A-48B7-433F-9DAB-0EC79D8016BB}"/>
+    <hyperlink ref="D14" r:id="rId15" xr:uid="{04F48E16-8194-4B60-BB88-B3DF93BB060F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cheat sheet version 1.7 by acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\2-Python-cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14F9927-A093-4E1C-9776-38200ACDCDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C32C9D0-AA6D-4C38-95B7-EF7CCA087677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Various" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="510">
   <si>
     <t>string-&gt;int</t>
   </si>
@@ -1079,9 +1079,6 @@
     <t>Dictionaries</t>
   </si>
   <si>
-    <t>my_dict={"Alex":(1,2,3)}</t>
-  </si>
-  <si>
     <t>can contain tuples, lists, sets, dictionaries</t>
   </si>
   <si>
@@ -1169,9 +1166,6 @@
     <t>A dead simple, responsive boilerplate.</t>
   </si>
   <si>
-    <t>Python Basics Cheat Sheet version 1.6</t>
-  </si>
-  <si>
     <t>a,b=(1,2)</t>
   </si>
   <si>
@@ -1433,9 +1427,6 @@
     <t>dictionary.update({key1: value2})</t>
   </si>
   <si>
-    <t>removes last key/value pair</t>
-  </si>
-  <si>
     <t>dictionary.copy()</t>
   </si>
   <si>
@@ -1478,12 +1469,6 @@
     <t>Tuples</t>
   </si>
   <si>
-    <t>immutable</t>
-  </si>
-  <si>
-    <t>text="test" if True else "ready"</t>
-  </si>
-  <si>
     <t>my_tuple=(1,"Alex", "Rose", 5)</t>
   </si>
   <si>
@@ -1496,15 +1481,9 @@
     <t>my_tuple.index(element)</t>
   </si>
   <si>
-    <t>returns index of element</t>
-  </si>
-  <si>
     <t>my_tuple.count(element)</t>
   </si>
   <si>
-    <t>counts number of elements in tuple</t>
-  </si>
-  <si>
     <t>[(1,2),2] or ([1,2],2)</t>
   </si>
   <si>
@@ -1548,6 +1527,171 @@
   </si>
   <si>
     <t>a,b,c=(1,2,3)</t>
+  </si>
+  <si>
+    <t>Sets</t>
+  </si>
+  <si>
+    <t>my_set={'Orange','Kiwi'}</t>
+  </si>
+  <si>
+    <t>set((1,2,3)) set([1,2,3])</t>
+  </si>
+  <si>
+    <t>can be created from list, tuple, dictionary, range</t>
+  </si>
+  <si>
+    <t>len(my_set)</t>
+  </si>
+  <si>
+    <t>length of set</t>
+  </si>
+  <si>
+    <t>my_set.add('Potato')</t>
+  </si>
+  <si>
+    <t>to add element to the end</t>
+  </si>
+  <si>
+    <t>my_set.clear()</t>
+  </si>
+  <si>
+    <t>removes all elements</t>
+  </si>
+  <si>
+    <t>my_set.copy()</t>
+  </si>
+  <si>
+    <t>copy the set</t>
+  </si>
+  <si>
+    <t>my_set.discard(element)</t>
+  </si>
+  <si>
+    <t>removes element from set</t>
+  </si>
+  <si>
+    <t>check if element in set</t>
+  </si>
+  <si>
+    <t>my_set.update(['Apple', 'Grapes'])</t>
+  </si>
+  <si>
+    <t>adding more elements to set</t>
+  </si>
+  <si>
+    <t>my_set{1,2, (1,5)}</t>
+  </si>
+  <si>
+    <t>can contain tuples</t>
+  </si>
+  <si>
+    <t>frosenset({4,5,6})</t>
+  </si>
+  <si>
+    <t>can be inside the set</t>
+  </si>
+  <si>
+    <t>my_set | my_set1</t>
+  </si>
+  <si>
+    <t>union -&gt; all elements from two sets and removes any duplicates</t>
+  </si>
+  <si>
+    <t>my_set &amp; my_set2</t>
+  </si>
+  <si>
+    <t>intersection-&gt;find common elements in two sets</t>
+  </si>
+  <si>
+    <t>my_set - my_set3</t>
+  </si>
+  <si>
+    <t>difference-&gt;difference between sets</t>
+  </si>
+  <si>
+    <t>my_set ^ my_set4</t>
+  </si>
+  <si>
+    <t>symmetric difference-&gt;all unique elements in two sets</t>
+  </si>
+  <si>
+    <t>my_set=set(my_list)</t>
+  </si>
+  <si>
+    <t>returns set without duplicate elements</t>
+  </si>
+  <si>
+    <t>my_set.difference(other_set)</t>
+  </si>
+  <si>
+    <t>difference between sets</t>
+  </si>
+  <si>
+    <t>my_set.difference_update(other_set)</t>
+  </si>
+  <si>
+    <t>removes all elements of other set from this set</t>
+  </si>
+  <si>
+    <t>my_set.intersection(other_set)</t>
+  </si>
+  <si>
+    <t>find common elements in two sets</t>
+  </si>
+  <si>
+    <t>my_set.isdisjoint(other_set)</t>
+  </si>
+  <si>
+    <t>True / False anything in common between sets</t>
+  </si>
+  <si>
+    <t>my_set.union(other_set)</t>
+  </si>
+  <si>
+    <t>new set from two sets, removes duplicates</t>
+  </si>
+  <si>
+    <t>my_set.issubset(other_set)</t>
+  </si>
+  <si>
+    <t>True / False elements from my_set are in other set</t>
+  </si>
+  <si>
+    <t>other_set.issuperset(my_set)</t>
+  </si>
+  <si>
+    <t>True/False other set has elements of my set</t>
+  </si>
+  <si>
+    <t>if "Alex" in my_set:</t>
+  </si>
+  <si>
+    <t>returns the number of times a specified value occurs in a tuple</t>
+  </si>
+  <si>
+    <t>searches the tuple for a specified value and returns the position of where it was found</t>
+  </si>
+  <si>
+    <t>my_dict={"Alex":(1,2,3),(1,2):'Alex'}</t>
+  </si>
+  <si>
+    <t>removes the last inserted key-value pair</t>
+  </si>
+  <si>
+    <t>Python Cheat Sheet version 1.7</t>
+  </si>
+  <si>
+    <t>input(element) - gets input from user as string</t>
+  </si>
+  <si>
+    <t>immutable / have unique elements, removes duplicates</t>
+  </si>
+  <si>
+    <t>immutable,can not sort and reverse</t>
+  </si>
+  <si>
+    <t>if 'Orange' in my_set</t>
   </si>
 </sst>
 </file>
@@ -1653,7 +1797,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1674,6 +1818,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1994,8 +2140,8 @@
   </sheetPr>
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,7 +2159,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>335</v>
+        <v>505</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2058,7 +2204,7 @@
         <v>222</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>232</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2072,7 +2218,7 @@
         <v>223</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>181</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2082,6 +2228,9 @@
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
         <v>224</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2129,7 +2278,7 @@
         <v>176</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>227</v>
@@ -2149,13 +2298,13 @@
         <v>177</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>228</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2169,7 +2318,7 @@
         <v>229</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2420,7 +2569,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>245</v>
@@ -2433,7 +2582,7 @@
       </c>
       <c r="B46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2444,7 +2593,7 @@
         <v>286</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2455,7 +2604,7 @@
         <v>284</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2466,7 +2615,7 @@
         <v>282</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2477,7 +2626,7 @@
         <v>280</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2488,7 +2637,7 @@
         <v>278</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2796,10 +2945,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2810,9 +2959,11 @@
     <col min="4" max="4" width="53.42578125" customWidth="1"/>
     <col min="5" max="5" width="48" customWidth="1"/>
     <col min="6" max="6" width="1" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>165</v>
       </c>
@@ -2820,11 +2971,14 @@
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>164</v>
       </c>
@@ -2835,10 +2989,16 @@
         <v>304</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>75</v>
       </c>
@@ -2846,13 +3006,17 @@
         <v>289</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>456</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>127</v>
       </c>
@@ -2860,13 +3024,19 @@
         <v>128</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="16" t="s">
+        <v>457</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>132</v>
       </c>
@@ -2874,13 +3044,19 @@
         <v>133</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>97</v>
       </c>
@@ -2888,25 +3064,37 @@
         <v>98</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>463</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
@@ -2914,13 +3102,19 @@
         <v>77</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>465</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>78</v>
       </c>
@@ -2928,13 +3122,19 @@
         <v>79</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>80</v>
       </c>
@@ -2942,13 +3142,19 @@
         <v>81</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>82</v>
       </c>
@@ -2956,13 +3162,19 @@
         <v>83</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>470</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
@@ -2970,13 +3182,19 @@
         <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>472</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>110</v>
       </c>
@@ -2984,13 +3202,19 @@
         <v>111</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>129</v>
       </c>
@@ -2998,13 +3222,19 @@
         <v>131</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>476</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>88</v>
       </c>
@@ -3012,13 +3242,19 @@
         <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>478</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>94</v>
       </c>
@@ -3026,13 +3262,19 @@
         <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>292</v>
       </c>
@@ -3040,13 +3282,19 @@
         <v>293</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>482</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>108</v>
       </c>
@@ -3054,13 +3302,19 @@
         <v>109</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
@@ -3068,13 +3322,19 @@
         <v>130</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>100</v>
       </c>
@@ -3082,13 +3342,19 @@
         <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>488</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>90</v>
       </c>
@@ -3096,13 +3362,19 @@
         <v>91</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>92</v>
       </c>
@@ -3110,13 +3382,19 @@
         <v>93</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>104</v>
       </c>
@@ -3124,13 +3402,19 @@
         <v>105</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>106</v>
       </c>
@@ -3138,11 +3422,17 @@
         <v>107</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>294</v>
       </c>
@@ -3150,21 +3440,33 @@
         <v>113</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>117</v>
       </c>
@@ -3172,30 +3474,28 @@
         <v>118</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>119</v>
       </c>
@@ -3203,13 +3503,13 @@
         <v>120</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>121</v>
       </c>
@@ -3223,7 +3523,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>123</v>
       </c>
@@ -3231,10 +3531,10 @@
         <v>124</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>446</v>
+        <v>502</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3245,10 +3545,10 @@
         <v>126</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>113</v>
+        <v>501</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3259,10 +3559,10 @@
         <v>85</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>449</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3273,10 +3573,10 @@
         <v>87</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3287,35 +3587,39 @@
         <v>115</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D37" s="16" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>459</v>
-      </c>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="1"/>
+      <c r="E40" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3349,27 +3653,27 @@
         <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E1" s="6"/>
       <c r="G1" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B2" s="6"/>
       <c r="D2" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3380,13 +3684,13 @@
         <v>71</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3409,7 +3713,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3422,7 +3726,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3590,7 +3894,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -3602,7 +3906,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>159</v>
@@ -3649,10 +3953,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A25:A26"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3666,204 +3970,232 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B1" s="6"/>
       <c r="D1" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="E9" s="1" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="D13" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="D14" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="D15" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="D16" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="D17" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>376</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>404</v>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -3880,7 +4212,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3946,10 +4278,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>184</v>
@@ -3970,10 +4302,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>194</v>
@@ -3984,24 +4316,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>388</v>
-      </c>
       <c r="D8" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>334</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>387</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>389</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -4038,18 +4370,18 @@
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="D14" s="10" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B16" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -4069,6 +4401,7 @@
     <hyperlink ref="A8" r:id="rId13" xr:uid="{23507FA9-2015-4A48-9B33-9831ED449069}"/>
     <hyperlink ref="A7" r:id="rId14" xr:uid="{65E1EF1A-48B7-433F-9DAB-0EC79D8016BB}"/>
     <hyperlink ref="D14" r:id="rId15" xr:uid="{04F48E16-8194-4B60-BB88-B3DF93BB060F}"/>
+    <hyperlink ref="A9" r:id="rId16" xr:uid="{97D7A46C-69C6-4EBE-9F71-17AF79DB53E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cheat sheet version 1.8 by acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\2-Python-cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C32C9D0-AA6D-4C38-95B7-EF7CCA087677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA85822D-334F-4DB9-95A2-12BD78A691A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Various" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="532">
   <si>
     <t>string-&gt;int</t>
   </si>
@@ -539,9 +539,6 @@
     <t xml:space="preserve">     do something</t>
   </si>
   <si>
-    <t>break, continue, pass</t>
-  </si>
-  <si>
     <t>Ternary operator</t>
   </si>
   <si>
@@ -1679,9 +1676,6 @@
     <t>removes the last inserted key-value pair</t>
   </si>
   <si>
-    <t>Python Cheat Sheet version 1.7</t>
-  </si>
-  <si>
     <t>input(element) - gets input from user as string</t>
   </si>
   <si>
@@ -1692,13 +1686,315 @@
   </si>
   <si>
     <t>if 'Orange' in my_set</t>
+  </si>
+  <si>
+    <t>We use "truthy" and "falsy" to differentiate from the bool values True and False. A "truthy" value will satisfy the check performed by if or while statements. As explained in the documentation, all values are considered "truthy" except for the following, which are "falsy":</t>
+  </si>
+  <si>
+    <t>Numbers that are numerically equal to zero, including:</t>
+  </si>
+  <si>
+    <t>0j</t>
+  </si>
+  <si>
+    <t>decimal.Decimal(0)</t>
+  </si>
+  <si>
+    <t>fraction.Fraction(0, 1)</t>
+  </si>
+  <si>
+    <t>Empty sequences and collections, including:</t>
+  </si>
+  <si>
+    <r>
+      <t>[]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> - an empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>list</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> - an empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>dict</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> - an empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>tuple</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>set()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> - an empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>set</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> - an empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>str</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> - an empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>bytes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>bytearray(b'')</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> - an empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>bytearray</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>memoryview(b'')</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> - an empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>memoryview</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>an empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>, like </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>range(0)</t>
+    </r>
+  </si>
+  <si>
+    <t>objects for which</t>
+  </si>
+  <si>
+    <r>
+      <t>obj.__bool__()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> returns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>False</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>obj.__len__()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> returns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>, given that </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF232629"/>
+        <rFont val="Var(--ff-mono)"/>
+      </rPr>
+      <t>obj.__bool__</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> is undefined</t>
+    </r>
+  </si>
+  <si>
+    <t>Truthy and falsy</t>
+  </si>
+  <si>
+    <t>can be used break, continue, pass</t>
+  </si>
+  <si>
+    <t>if 'hit' in tuple: do something</t>
+  </si>
+  <si>
+    <t>if 'hit' in set: do something</t>
+  </si>
+  <si>
+    <t>if 'hit' in dictionary: do something</t>
+  </si>
+  <si>
+    <t>Python Cheat Sheet version 1.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1741,6 +2037,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF232629"/>
+      <name val="Var(--ff-mono)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF232629"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1797,7 +2103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1820,6 +2126,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2140,11 +2461,11 @@
   </sheetPr>
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
@@ -2157,18 +2478,18 @@
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>505</v>
+        <v>531</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="F1" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>74</v>
       </c>
@@ -2176,307 +2497,307 @@
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="F2" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="5.25" customHeight="1"/>
+    <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="6"/>
       <c r="D8" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F9" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" s="1" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="5.25" customHeight="1"/>
+    <row r="20" spans="1:6">
+      <c r="A20" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="5.25" customHeight="1"/>
+    <row r="32" spans="1:6">
+      <c r="A32" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>269</v>
       </c>
       <c r="B32" s="6"/>
       <c r="F32" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
@@ -2487,7 +2808,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
@@ -2495,23 +2816,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -2519,141 +2840,141 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:6">
+      <c r="A40" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="B43" s="1" t="s">
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="5.25" customHeight="1"/>
+    <row r="46" spans="1:6">
       <c r="A46" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2673,21 +2994,21 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
@@ -2695,7 +3016,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2703,7 +3024,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2711,15 +3032,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -2727,15 +3048,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2743,7 +3064,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -2751,7 +3072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -2759,7 +3080,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -2767,7 +3088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -2775,7 +3096,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -2783,7 +3104,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -2791,7 +3112,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -2799,23 +3120,23 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -2823,7 +3144,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -2831,7 +3152,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -2839,15 +3160,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -2855,7 +3176,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -2863,7 +3184,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
@@ -2871,7 +3192,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -2879,7 +3200,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -2887,7 +3208,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="7" t="s">
         <v>51</v>
       </c>
@@ -2895,7 +3216,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
@@ -2903,7 +3224,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
@@ -2911,7 +3232,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
@@ -2919,7 +3240,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -2927,7 +3248,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -2947,11 +3268,11 @@
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38.85546875" customWidth="1"/>
     <col min="2" max="2" width="45.5703125" customWidth="1"/>
@@ -2963,9 +3284,9 @@
     <col min="8" max="8" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2975,48 +3296,48 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="6.75" customHeight="1">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>127</v>
       </c>
@@ -3024,19 +3345,19 @@
         <v>128</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G5" s="16" t="s">
+        <v>456</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>132</v>
       </c>
@@ -3044,19 +3365,19 @@
         <v>133</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="G6" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>97</v>
       </c>
@@ -3064,37 +3385,37 @@
         <v>98</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G7" s="16" t="s">
+        <v>460</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G8" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
@@ -3102,19 +3423,19 @@
         <v>77</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G9" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>78</v>
       </c>
@@ -3122,19 +3443,19 @@
         <v>79</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>417</v>
-      </c>
       <c r="G10" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>80</v>
       </c>
@@ -3142,19 +3463,19 @@
         <v>81</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>82</v>
       </c>
@@ -3162,19 +3483,19 @@
         <v>83</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G12" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
@@ -3182,19 +3503,19 @@
         <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G13" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>110</v>
       </c>
@@ -3202,19 +3523,19 @@
         <v>111</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G14" s="16" t="s">
+        <v>473</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>129</v>
       </c>
@@ -3222,19 +3543,19 @@
         <v>131</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G15" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>88</v>
       </c>
@@ -3242,19 +3563,19 @@
         <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G16" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>94</v>
       </c>
@@ -3262,39 +3583,39 @@
         <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="G17" s="16" t="s">
-        <v>480</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="G18" s="16" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="G18" s="16" t="s">
+      <c r="H18" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>108</v>
       </c>
@@ -3302,19 +3623,19 @@
         <v>109</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G19" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
@@ -3322,19 +3643,19 @@
         <v>130</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G20" s="16" t="s">
+        <v>485</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>100</v>
       </c>
@@ -3342,19 +3663,19 @@
         <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G21" s="16" t="s">
+        <v>487</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>90</v>
       </c>
@@ -3362,19 +3683,19 @@
         <v>91</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="G22" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>92</v>
       </c>
@@ -3382,19 +3703,19 @@
         <v>93</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>319</v>
-      </c>
       <c r="G23" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>104</v>
       </c>
@@ -3402,19 +3723,19 @@
         <v>105</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>423</v>
-      </c>
       <c r="G24" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>106</v>
       </c>
@@ -3422,51 +3743,51 @@
         <v>107</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E25" s="1"/>
       <c r="G25" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G26" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>117</v>
       </c>
@@ -3474,28 +3795,28 @@
         <v>118</v>
       </c>
       <c r="D28" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>434</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>435</v>
-      </c>
       <c r="E29" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>119</v>
       </c>
@@ -3503,13 +3824,13 @@
         <v>120</v>
       </c>
       <c r="D30" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>121</v>
       </c>
@@ -3517,13 +3838,13 @@
         <v>122</v>
       </c>
       <c r="D31" s="16" t="s">
+        <v>442</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>123</v>
       </c>
@@ -3531,13 +3852,13 @@
         <v>124</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>125</v>
       </c>
@@ -3545,13 +3866,13 @@
         <v>126</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>84</v>
       </c>
@@ -3559,13 +3880,13 @@
         <v>85</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>86</v>
       </c>
@@ -3573,13 +3894,13 @@
         <v>87</v>
       </c>
       <c r="D35" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>114</v>
       </c>
@@ -3587,37 +3908,37 @@
         <v>115</v>
       </c>
       <c r="D36" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="E36" s="1" t="s">
+    </row>
+    <row r="37" spans="1:5">
+      <c r="D37" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="D38" s="16" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D37" s="16" t="s">
-        <v>441</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D38" s="16" t="s">
+      <c r="E38" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5">
       <c r="D39" s="16" t="s">
+        <v>444</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5">
       <c r="D40" s="1"/>
       <c r="E40" s="19"/>
     </row>
@@ -3638,7 +3959,7 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
@@ -3648,35 +3969,35 @@
     <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E1" s="6"/>
       <c r="G1" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B2" s="6"/>
       <c r="D2" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
@@ -3684,16 +4005,16 @@
         <v>71</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>65</v>
       </c>
@@ -3703,7 +4024,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>66</v>
       </c>
@@ -3713,10 +4034,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>68</v>
       </c>
@@ -3726,10 +4047,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
@@ -3739,7 +4060,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>135</v>
       </c>
@@ -3760,13 +4081,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="1.140625" customWidth="1"/>
@@ -3777,21 +4098,21 @@
     <col min="7" max="7" width="47.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>146</v>
       </c>
@@ -3802,10 +4123,10 @@
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>148</v>
       </c>
@@ -3815,10 +4136,13 @@
       <c r="E3" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="5" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>156</v>
@@ -3826,8 +4150,11 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="20" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>137</v>
       </c>
@@ -3837,8 +4164,9 @@
       <c r="E5" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>138</v>
       </c>
@@ -3848,8 +4176,9 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>137</v>
       </c>
@@ -3859,90 +4188,187 @@
       <c r="E7" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>161</v>
+        <v>527</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="21" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>137</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.5">
       <c r="A12" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="G13" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+      <c r="G14" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G18" s="22" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G19" s="23" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
-        <v>161</v>
+        <v>527</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="G21" s="23" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="G22" s="23" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="G23" s="23" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="G24" s="23" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="G25" s="23" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="G26" s="23" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="G27" s="24" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="G28" s="22" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="G29" s="23" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.5">
+      <c r="G30" s="23" t="s">
+        <v>525</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G4:G9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3959,7 +4385,7 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
@@ -3968,234 +4394,234 @@
     <col min="5" max="5" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B1" s="6"/>
       <c r="D1" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="D5" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="D7" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="D9" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="D12" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="D13" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="D14" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="D15" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="D16" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="D17" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -4215,7 +4641,7 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="2" width="67.140625" customWidth="1"/>
@@ -4224,164 +4650,164 @@
     <col min="5" max="5" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B1" s="6"/>
       <c r="D1" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>134</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>258</v>
-      </c>
       <c r="D3" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>271</v>
-      </c>
       <c r="D4" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>382</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>383</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="D6" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>389</v>
-      </c>
       <c r="D7" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B9" s="12" t="s">
         <v>386</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>387</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="D14" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>406</v>
+      </c>
+      <c r="B16" t="s">
         <v>407</v>
-      </c>
-      <c r="B16" t="s">
-        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cheat sheet version 1.9 by acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\2-Python-cheatsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA85822D-334F-4DB9-95A2-12BD78A691A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A096288-3734-413A-AE4B-2409F06038AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Various" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Loops Conditions Ternary operat" sheetId="6" r:id="rId5"/>
     <sheet name="Command prompt Terminal command" sheetId="7" r:id="rId6"/>
     <sheet name="Links" sheetId="2" r:id="rId7"/>
+    <sheet name="Terms" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="579">
   <si>
     <t>string-&gt;int</t>
   </si>
@@ -539,9 +540,6 @@
     <t xml:space="preserve">     do something</t>
   </si>
   <si>
-    <t>Ternary operator</t>
-  </si>
-  <si>
     <r>
       <t>condition_if_true</t>
     </r>
@@ -1106,9 +1104,6 @@
     <t>list of key and value pairs</t>
   </si>
   <si>
-    <t>iterate through dictionary</t>
-  </si>
-  <si>
     <t>my_dict["Alex"][1]-&gt;2</t>
   </si>
   <si>
@@ -1451,9 +1446,6 @@
     <t>dictionary.items()</t>
   </si>
   <si>
-    <t>for key in dictionary:</t>
-  </si>
-  <si>
     <t>if "key" not in dictionary:</t>
   </si>
   <si>
@@ -1619,16 +1611,7 @@
     <t>returns set without duplicate elements</t>
   </si>
   <si>
-    <t>my_set.difference(other_set)</t>
-  </si>
-  <si>
-    <t>difference between sets</t>
-  </si>
-  <si>
     <t>my_set.difference_update(other_set)</t>
-  </si>
-  <si>
-    <t>removes all elements of other set from this set</t>
   </si>
   <si>
     <t>my_set.intersection(other_set)</t>
@@ -1987,14 +1970,173 @@
     <t>if 'hit' in dictionary: do something</t>
   </si>
   <si>
-    <t>Python Cheat Sheet version 1.8</t>
+    <t>python manage.py runserver</t>
+  </si>
+  <si>
+    <t>pip install opencv-python</t>
+  </si>
+  <si>
+    <t>pip install opencv-contrib-python</t>
+  </si>
+  <si>
+    <t>Ctrl+C to quit</t>
+  </si>
+  <si>
+    <t>Django installation and use</t>
+  </si>
+  <si>
+    <t>Flask installation</t>
+  </si>
+  <si>
+    <t>OpenCV installation</t>
+  </si>
+  <si>
+    <t>difference between sets or set and list</t>
+  </si>
+  <si>
+    <t>my_set.difference(other_set or list)</t>
+  </si>
+  <si>
+    <t>removes same elements existing in other set from this set</t>
+  </si>
+  <si>
+    <t>my_set.pop()</t>
+  </si>
+  <si>
+    <t>Removes the specified element</t>
+  </si>
+  <si>
+    <t>Removes first element from the set</t>
+  </si>
+  <si>
+    <t>my_set.remove('Kiwi')</t>
+  </si>
+  <si>
+    <t>Removes the items in this set that are not present in other specified set</t>
+  </si>
+  <si>
+    <t>my_set.intersection_update(other_set)</t>
+  </si>
+  <si>
+    <t>Ternary operator/Conditional expression</t>
+  </si>
+  <si>
+    <t>True and True</t>
+  </si>
+  <si>
+    <t>False and True</t>
+  </si>
+  <si>
+    <t>True and False</t>
+  </si>
+  <si>
+    <t>False and False</t>
+  </si>
+  <si>
+    <t>True or True</t>
+  </si>
+  <si>
+    <t>False or True</t>
+  </si>
+  <si>
+    <t>True or False</t>
+  </si>
+  <si>
+    <t>False or False</t>
+  </si>
+  <si>
+    <t>Short circuting / logical operator AND</t>
+  </si>
+  <si>
+    <t>Short circuting / logical operator OR</t>
+  </si>
+  <si>
+    <t>Keyword IS</t>
+  </si>
+  <si>
+    <t>Checks if location in memory is the same</t>
+  </si>
+  <si>
+    <t>10 is 10.0 -&gt; False</t>
+  </si>
+  <si>
+    <t>Iterable</t>
+  </si>
+  <si>
+    <t>Iterate</t>
+  </si>
+  <si>
+    <t>List, dictionary, tuple, set, string</t>
+  </si>
+  <si>
+    <t>One by one check each item in the collection</t>
+  </si>
+  <si>
+    <t>Terms used in Python</t>
+  </si>
+  <si>
+    <t>http://www.pythontutor.com/</t>
+  </si>
+  <si>
+    <t>for item in dictionary:</t>
+  </si>
+  <si>
+    <t>iterate through dictionary keys</t>
+  </si>
+  <si>
+    <t>for value in dictionary.values():</t>
+  </si>
+  <si>
+    <t>iterate through dictionary values</t>
+  </si>
+  <si>
+    <t>for key in dictionary.keys():</t>
+  </si>
+  <si>
+    <t>for item in dictionary.items():</t>
+  </si>
+  <si>
+    <t>iterate through dictionary key/value pairs -&gt;tuples</t>
+  </si>
+  <si>
+    <t>if key not in dictionary True/False</t>
+  </si>
+  <si>
+    <t>for key,value in dictionary.items():</t>
+  </si>
+  <si>
+    <t>dictionary unpacking</t>
+  </si>
+  <si>
+    <t>for _ in range(10,0,-1): # not including 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       print(_)</t>
+  </si>
+  <si>
+    <t>PySimpleGUI</t>
+  </si>
+  <si>
+    <t>from random import randint,choice</t>
+  </si>
+  <si>
+    <t>Imported randint and choice functions</t>
+  </si>
+  <si>
+    <t>Python GUIs for Humans</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/PySimpleGUI/</t>
+  </si>
+  <si>
+    <t>Python Cheat Sheet version 1.9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2048,6 +2190,13 @@
       <color rgb="FF232629"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2075,7 +2224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2083,27 +2232,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2116,19 +2250,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2140,6 +2264,11 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2459,10 +2588,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2480,13 +2609,13 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>531</v>
+        <v>578</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="F1" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2497,7 +2626,7 @@
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="F2" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2505,41 +2634,41 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2548,249 +2677,258 @@
       </c>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="5.25" customHeight="1"/>
     <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" s="6"/>
       <c r="D8" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>552</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>553</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>554</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="5.25" customHeight="1"/>
     <row r="20" spans="1:6">
       <c r="A20" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="5.25" customHeight="1"/>
     <row r="32" spans="1:6">
       <c r="A32" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B32" s="6"/>
       <c r="F32" s="1" t="s">
@@ -2818,15 +2956,15 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>8</v>
@@ -2845,136 +2983,213 @@
         <v>112</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="5.25" customHeight="1"/>
     <row r="46" spans="1:6">
       <c r="A46" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>338</v>
+        <v>284</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>336</v>
+        <v>280</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>334</v>
+        <v>276</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="5.25" customHeight="1"/>
+    <row r="55" spans="1:4">
+      <c r="A55" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B56" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B57" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B58" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B59" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="B60" s="6"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B61" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B62" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B63" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B64" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3005,7 +3220,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3034,10 +3249,10 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3053,7 +3268,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3125,15 +3340,15 @@
         <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3162,10 +3377,10 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3266,10 +3481,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3286,7 +3501,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -3301,22 +3516,22 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3324,16 +3539,16 @@
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>455</v>
+        <v>318</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>452</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -3345,16 +3560,16 @@
         <v>128</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>456</v>
+        <v>303</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>453</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3365,16 +3580,16 @@
         <v>133</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>458</v>
+      <c r="G6" s="1" t="s">
+        <v>455</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3385,16 +3600,16 @@
         <v>98</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>460</v>
+        <v>306</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>457</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3403,16 +3618,16 @@
       </c>
       <c r="B8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>462</v>
+        <v>320</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>459</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3423,16 +3638,16 @@
         <v>77</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>464</v>
+        <v>319</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>461</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3443,16 +3658,16 @@
         <v>79</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>466</v>
+        <v>414</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>463</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3463,16 +3678,16 @@
         <v>81</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>507</v>
+        <v>307</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>501</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3483,16 +3698,16 @@
         <v>83</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>469</v>
+        <v>429</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>466</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3503,16 +3718,16 @@
         <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>471</v>
+        <v>308</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>468</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3523,16 +3738,16 @@
         <v>111</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>473</v>
+        <v>317</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>470</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -3543,16 +3758,16 @@
         <v>131</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>475</v>
+        <v>309</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>472</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -3563,16 +3778,16 @@
         <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>477</v>
+        <v>310</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>474</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -3583,36 +3798,36 @@
         <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>479</v>
+        <v>311</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>476</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>292</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>481</v>
+        <v>312</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>478</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -3623,16 +3838,16 @@
         <v>109</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>483</v>
+        <v>408</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>480</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -3643,16 +3858,16 @@
         <v>130</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>485</v>
+        <v>497</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>533</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>486</v>
+        <v>532</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -3663,16 +3878,16 @@
         <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>487</v>
+        <v>307</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>482</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>488</v>
+        <v>534</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -3683,16 +3898,16 @@
         <v>91</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>489</v>
+        <v>314</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>483</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -3703,16 +3918,16 @@
         <v>93</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>491</v>
+        <v>316</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>485</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -3723,16 +3938,16 @@
         <v>105</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>493</v>
+        <v>420</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>487</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -3743,34 +3958,36 @@
         <v>107</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="G25" s="16" t="s">
-        <v>495</v>
+        <v>427</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>489</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>429</v>
+        <v>561</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>497</v>
+        <v>562</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>491</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -3778,13 +3995,19 @@
         <v>116</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>499</v>
+        <v>322</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>493</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -3794,26 +4017,37 @@
       <c r="B28" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="G28" s="17"/>
+      <c r="D28" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>434</v>
+        <v>339</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>566</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>452</v>
+        <v>567</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -3823,11 +4057,17 @@
       <c r="B30" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="16" t="s">
-        <v>435</v>
+      <c r="D30" s="1" t="s">
+        <v>569</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>436</v>
+        <v>570</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -3837,12 +4077,6 @@
       <c r="B31" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="16" t="s">
-        <v>442</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>443</v>
-      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -3851,96 +4085,139 @@
       <c r="B32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D32" s="16" t="s">
-        <v>437</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="16" t="s">
-        <v>438</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D34" s="16" t="s">
-        <v>439</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="16" t="s">
-        <v>450</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="16" t="s">
+    </row>
+    <row r="37" spans="1:2" ht="6" customHeight="1"/>
+    <row r="38" spans="1:2">
+      <c r="A38" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="D37" s="16" t="s">
-        <v>440</v>
-      </c>
-      <c r="E37" s="1" t="s">
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="D38" s="16" t="s">
-        <v>448</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="D39" s="16" t="s">
-        <v>444</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="D40" s="1"/>
-      <c r="E40" s="19"/>
+      <c r="B49" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3953,10 +4230,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3964,7 +4241,7 @@
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="1.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
     <col min="5" max="5" width="34.85546875" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
@@ -3974,27 +4251,27 @@
         <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E1" s="6"/>
       <c r="G1" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B2" s="6"/>
       <c r="D2" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4005,13 +4282,13 @@
         <v>71</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4021,8 +4298,12 @@
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
@@ -4034,7 +4315,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4047,7 +4328,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -4069,6 +4350,28 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4084,7 +4387,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4109,7 +4412,7 @@
         <v>157</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>161</v>
+        <v>541</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4123,7 +4426,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4137,12 +4440,12 @@
         <v>160</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>156</v>
@@ -4150,8 +4453,8 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>508</v>
+      <c r="G4" s="19" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4164,11 +4467,11 @@
       <c r="E5" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>138</v>
+        <v>571</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>151</v>
@@ -4176,11 +4479,11 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="20"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>137</v>
+        <v>572</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>152</v>
@@ -4188,36 +4491,36 @@
       <c r="E7" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="G9" s="20"/>
+        <v>521</v>
+      </c>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>247</v>
+        <v>13</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4227,19 +4530,19 @@
       <c r="E11" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G11" s="21" t="b">
+      <c r="G11" s="13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.5">
       <c r="A12" s="1" t="s">
-        <v>343</v>
+        <v>139</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G12" s="22" t="s">
-        <v>509</v>
+      <c r="G12" s="14" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4247,20 +4550,20 @@
         <v>137</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="G13" s="23">
+        <v>522</v>
+      </c>
+      <c r="G13" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="G14" s="23">
+        <v>523</v>
+      </c>
+      <c r="G14" s="15">
         <v>0</v>
       </c>
     </row>
@@ -4269,100 +4572,106 @@
         <v>137</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>510</v>
+        <v>524</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>140</v>
+        <v>342</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>513</v>
+        <v>140</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G21" s="15" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="G23" s="15" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="G24" s="15" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="G25" s="15" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="G20" s="23" t="s">
+    <row r="26" spans="1:7">
+      <c r="G26" s="15" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="G21" s="23" t="s">
+    <row r="27" spans="1:7">
+      <c r="G27" s="16" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="G22" s="23" t="s">
+    <row r="28" spans="1:7">
+      <c r="G28" s="14" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="G23" s="23" t="s">
+    <row r="29" spans="1:7">
+      <c r="G29" s="15" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="G24" s="23" t="s">
+    <row r="30" spans="1:7" ht="28.5">
+      <c r="G30" s="15" t="s">
         <v>519</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="G25" s="23" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="G26" s="23" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="G27" s="24" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="G28" s="22" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="G29" s="23" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="28.5">
-      <c r="G30" s="23" t="s">
-        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -4379,10 +4688,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4396,232 +4705,266 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B1" s="6"/>
       <c r="D1" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="D16" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="D17" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
+    <row r="18" spans="1:5" ht="6.75" customHeight="1"/>
     <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>393</v>
-      </c>
+      <c r="A19" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
+    </row>
+    <row r="22" spans="1:5" ht="6" customHeight="1"/>
     <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>401</v>
+      <c r="A23" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -4635,10 +4978,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4652,162 +4995,163 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="6"/>
       <c r="D1" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E2" s="11" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1"/>
+      <c r="D6" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="10" t="s">
+      <c r="E7" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="18" t="s">
         <v>381</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B8" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="D6" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="10" t="s">
+      <c r="B9" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>387</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="E14" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>385</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="10" t="s">
-        <v>384</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="D14" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>406</v>
-      </c>
-      <c r="B16" t="s">
-        <v>407</v>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>560</v>
       </c>
     </row>
   </sheetData>
@@ -4828,7 +5172,92 @@
     <hyperlink ref="A7" r:id="rId14" xr:uid="{65E1EF1A-48B7-433F-9DAB-0EC79D8016BB}"/>
     <hyperlink ref="D14" r:id="rId15" xr:uid="{04F48E16-8194-4B60-BB88-B3DF93BB060F}"/>
     <hyperlink ref="A9" r:id="rId16" xr:uid="{97D7A46C-69C6-4EBE-9F71-17AF79DB53E4}"/>
+    <hyperlink ref="A14" r:id="rId17" xr:uid="{E93BFB77-DBB7-4BE4-A023-E05CECFB2970}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023B3C95-75DA-464A-BC00-472839EFFECB}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="40.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cheat sheet version 2.0 by acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A096288-3734-413A-AE4B-2409F06038AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED5C02-BA9E-4F91-BDAB-9CF09E613AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="582">
   <si>
     <t>string-&gt;int</t>
   </si>
@@ -489,12 +489,6 @@
     <t>print(I,char)</t>
   </si>
   <si>
-    <t>enumerate() can be used with</t>
-  </si>
-  <si>
-    <t>lists, tuples</t>
-  </si>
-  <si>
     <t>for item In list_of_items:</t>
   </si>
   <si>
@@ -2129,7 +2123,22 @@
     <t>https://pypi.org/project/PySimpleGUI/</t>
   </si>
   <si>
-    <t>Python Cheat Sheet version 1.9</t>
+    <t>Enumerate()</t>
+  </si>
+  <si>
+    <t>Can be used with itterables: string, list,tuple</t>
+  </si>
+  <si>
+    <t>Gives index</t>
+  </si>
+  <si>
+    <t>for i,char in enumerate("hello"):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  print(i,char)</t>
+  </si>
+  <si>
+    <t>Python Cheat Sheet version 2.0</t>
   </si>
 </sst>
 </file>
@@ -2591,7 +2600,7 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2609,13 +2618,13 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="F1" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2626,7 +2635,7 @@
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="F2" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2634,41 +2643,41 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2677,276 +2686,285 @@
       </c>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="5.25" customHeight="1"/>
     <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B8" s="6"/>
       <c r="D8" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>576</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>577</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="5.25" customHeight="1"/>
     <row r="20" spans="1:6">
       <c r="A20" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="5.25" customHeight="1"/>
     <row r="32" spans="1:6">
       <c r="A32" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B32" s="6"/>
-      <c r="F32" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
@@ -2954,23 +2972,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -2978,153 +2996,153 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="1" t="s">
+    <row r="42" spans="1:4">
+      <c r="A42" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="5.25" customHeight="1"/>
-    <row r="46" spans="1:6">
+    </row>
+    <row r="45" spans="1:4" ht="5.25" customHeight="1"/>
+    <row r="46" spans="1:4">
       <c r="A46" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="5.25" customHeight="1"/>
     <row r="55" spans="1:4">
       <c r="A55" s="5" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B55" s="5"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B56" s="1" t="b">
         <v>1</v>
@@ -3132,7 +3150,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B57" s="1" t="b">
         <v>0</v>
@@ -3140,7 +3158,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B58" s="1" t="b">
         <v>0</v>
@@ -3148,7 +3166,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B59" s="1" t="b">
         <v>0</v>
@@ -3156,13 +3174,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B60" s="6"/>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B61" s="1" t="b">
         <v>1</v>
@@ -3170,7 +3188,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B62" s="1" t="b">
         <v>1</v>
@@ -3178,7 +3196,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B63" s="1" t="b">
         <v>1</v>
@@ -3186,7 +3204,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B64" s="1" t="b">
         <v>0</v>
@@ -3220,7 +3238,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3249,10 +3267,10 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3268,7 +3286,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3340,15 +3358,15 @@
         <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3377,10 +3395,10 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3501,7 +3519,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -3516,22 +3534,22 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3539,16 +3557,16 @@
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -3560,16 +3578,16 @@
         <v>128</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3580,16 +3598,16 @@
         <v>133</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3600,16 +3618,16 @@
         <v>98</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3618,16 +3636,16 @@
       </c>
       <c r="B8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3638,16 +3656,16 @@
         <v>77</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3658,16 +3676,16 @@
         <v>79</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3678,16 +3696,16 @@
         <v>81</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3698,16 +3716,16 @@
         <v>83</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3718,16 +3736,16 @@
         <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3738,16 +3756,16 @@
         <v>111</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -3758,16 +3776,16 @@
         <v>131</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -3778,16 +3796,16 @@
         <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -3798,36 +3816,36 @@
         <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -3838,16 +3856,16 @@
         <v>109</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -3858,16 +3876,16 @@
         <v>130</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -3878,16 +3896,16 @@
         <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -3898,16 +3916,16 @@
         <v>91</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -3918,16 +3936,16 @@
         <v>93</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -3938,16 +3956,16 @@
         <v>105</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -3958,36 +3976,36 @@
         <v>107</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -3995,19 +4013,19 @@
         <v>116</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -4018,36 +4036,36 @@
         <v>118</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -4058,16 +4076,16 @@
         <v>120</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -4121,55 +4139,55 @@
     <row r="37" spans="1:2" ht="6" customHeight="1"/>
     <row r="38" spans="1:2">
       <c r="A38" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>113</v>
@@ -4177,42 +4195,42 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -4251,27 +4269,27 @@
         <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E1" s="6"/>
       <c r="G1" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B2" s="6"/>
       <c r="D2" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4282,13 +4300,13 @@
         <v>71</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>327</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4299,10 +4317,10 @@
         <v>72</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4315,7 +4333,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4328,7 +4346,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -4353,16 +4371,16 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4403,58 +4421,58 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>157</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4462,19 +4480,19 @@
         <v>137</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -4483,13 +4501,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G7" s="19"/>
     </row>
@@ -4498,7 +4516,7 @@
         <v>138</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E8" s="1"/>
       <c r="G8" s="19"/>
@@ -4508,10 +4526,10 @@
         <v>137</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="G9" s="19"/>
     </row>
@@ -4520,7 +4538,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4528,7 +4546,7 @@
         <v>137</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G11" s="13" t="b">
         <v>0</v>
@@ -4539,10 +4557,10 @@
         <v>139</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4550,7 +4568,7 @@
         <v>137</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="G13" s="15">
         <v>0</v>
@@ -4558,10 +4576,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="G14" s="15">
         <v>0</v>
@@ -4572,18 +4590,18 @@
         <v>137</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -4591,7 +4609,7 @@
         <v>137</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -4599,7 +4617,7 @@
         <v>140</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4607,7 +4625,7 @@
         <v>141</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4615,7 +4633,7 @@
         <v>142</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4623,55 +4641,55 @@
         <v>143</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="G23" s="15" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="G24" s="15" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="G25" s="15" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="G26" s="15" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="G27" s="16" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="G28" s="14" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="G29" s="15" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.5">
       <c r="G30" s="15" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -4705,266 +4723,266 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B1" s="6"/>
       <c r="D1" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="6.75" customHeight="1"/>
     <row r="19" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="6" customHeight="1"/>
     <row r="23" spans="1:5">
       <c r="A23" s="5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="5" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -4995,114 +5013,114 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B1" s="6"/>
       <c r="D1" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>189</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="18" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="18" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="D6" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="18" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>383</v>
-      </c>
       <c r="D8" s="18" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>384</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="1"/>
@@ -5127,31 +5145,31 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="18" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -5193,24 +5211,24 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>556</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
Cheatsheet version 3.3 by acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="882">
   <si>
     <t>string-&gt;int</t>
   </si>
@@ -2161,9 +2161,6 @@
     <t>.show()</t>
   </si>
   <si>
-    <t>Matplotlib.pyplot as plt</t>
-  </si>
-  <si>
     <t>plt.plot([1,2,3],[4,5,6])</t>
   </si>
   <si>
@@ -3160,17 +3157,32 @@
     <t>def test(a):</t>
   </si>
   <si>
-    <t>print(test.__doc__)</t>
-  </si>
-  <si>
-    <t>Python Cheat Sheet version 3.2</t>
+    <t>pathlib</t>
+  </si>
+  <si>
+    <t>Object-oriented filesystem paths</t>
+  </si>
+  <si>
+    <t>https://docs.python.org/3/library/pathlib.html</t>
+  </si>
+  <si>
+    <t>Matplotlib.pyplot</t>
+  </si>
+  <si>
+    <t>arguments-&gt;when call invoke function</t>
+  </si>
+  <si>
+    <t>parameters-&gt;when define function</t>
+  </si>
+  <si>
+    <t>Python Cheat Sheet version 3.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3252,8 +3264,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3281,12 +3302,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3334,22 +3349,22 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3671,7 +3686,7 @@
   <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3689,7 +3704,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -3712,10 +3727,10 @@
         <v>169</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>613</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3729,13 +3744,13 @@
         <v>214</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>667</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3752,10 +3767,10 @@
         <v>486</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3772,10 +3787,10 @@
         <v>225</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>866</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3788,12 +3803,6 @@
       </c>
       <c r="F6" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>870</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="5.25" customHeight="1"/>
@@ -3900,10 +3909,6 @@
       <c r="F13" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
@@ -3918,12 +3923,6 @@
       <c r="F14" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>803</v>
-      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
@@ -3933,16 +3932,10 @@
         <v>291</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>802</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3955,12 +3948,6 @@
       <c r="F16" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>804</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>806</v>
-      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
@@ -3980,34 +3967,18 @@
       <c r="B18" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="5.25" customHeight="1">
-      <c r="H19" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>818</v>
-      </c>
-    </row>
+    </row>
+    <row r="19" spans="1:9" ht="5.25" customHeight="1"/>
     <row r="20" spans="1:9">
       <c r="A20" s="5" t="s">
         <v>213</v>
       </c>
       <c r="B20" s="6"/>
       <c r="D20" s="5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -4018,16 +3989,10 @@
         <v>196</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>676</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>809</v>
+        <v>675</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -4038,16 +4003,10 @@
         <v>224</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>807</v>
-      </c>
-      <c r="I22" t="s">
-        <v>816</v>
+        <v>676</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -4058,16 +4017,10 @@
         <v>198</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>821</v>
+        <v>747</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="16.5" customHeight="1">
@@ -4077,17 +4030,11 @@
       <c r="B24" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D24" s="25" t="s">
-        <v>744</v>
+      <c r="D24" s="26" t="s">
+        <v>743</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>811</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>823</v>
+        <v>748</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -4097,12 +4044,9 @@
       <c r="B25" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D25" s="25"/>
+      <c r="D25" s="26"/>
       <c r="F25" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>820</v>
+        <v>749</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4112,11 +4056,11 @@
       <c r="B26" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D26" s="24" t="s">
-        <v>746</v>
+      <c r="D26" s="22" t="s">
+        <v>745</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -4127,13 +4071,10 @@
         <v>206</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>812</v>
+        <v>754</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -4143,11 +4084,11 @@
       <c r="B28" s="1" t="s">
         <v>208</v>
       </c>
+      <c r="D28" s="25" t="s">
+        <v>880</v>
+      </c>
       <c r="F28" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>813</v>
+        <v>750</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -4157,11 +4098,11 @@
       <c r="B29" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="D29" s="25" t="s">
+        <v>879</v>
+      </c>
       <c r="F29" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>815</v>
+        <v>751</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -4172,7 +4113,7 @@
         <v>212</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="5.25" customHeight="1"/>
@@ -4182,19 +4123,19 @@
       </c>
       <c r="B32" s="6"/>
       <c r="D32" s="5" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="H32" s="27" t="s">
-        <v>873</v>
-      </c>
-      <c r="I32" t="s">
+        <v>677</v>
+      </c>
+      <c r="H32" s="20" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" s="20" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
@@ -4202,16 +4143,17 @@
         <v>0</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="H33" s="27" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>678</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="I33" s="20"/>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
@@ -4219,16 +4161,19 @@
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="H34" s="23" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>679</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>869</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>255</v>
       </c>
@@ -4236,13 +4181,13 @@
         <v>232</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>231</v>
       </c>
@@ -4250,13 +4195,13 @@
         <v>8</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -4264,13 +4209,13 @@
         <v>4</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>111</v>
       </c>
@@ -4278,13 +4223,13 @@
         <v>233</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>769</v>
-      </c>
-      <c r="F38" s="23" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>768</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
         <v>226</v>
       </c>
@@ -4292,13 +4237,13 @@
         <v>234</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
         <v>230</v>
       </c>
@@ -4306,13 +4251,13 @@
         <v>229</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
         <v>236</v>
       </c>
@@ -4320,13 +4265,13 @@
         <v>235</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
         <v>228</v>
       </c>
@@ -4334,13 +4279,13 @@
         <v>227</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="9" t="s">
         <v>174</v>
       </c>
@@ -4348,13 +4293,13 @@
         <v>237</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
         <v>333</v>
       </c>
@@ -4362,14 +4307,14 @@
         <v>238</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="5.25" customHeight="1"/>
-    <row r="46" spans="1:8">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="5.25" customHeight="1"/>
+    <row r="46" spans="1:9">
       <c r="A46" s="5" t="s">
         <v>281</v>
       </c>
@@ -4378,10 +4323,10 @@
         <v>330</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>280</v>
       </c>
@@ -4392,10 +4337,10 @@
         <v>329</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
         <v>278</v>
       </c>
@@ -4406,7 +4351,7 @@
         <v>328</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -4420,7 +4365,7 @@
         <v>327</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -4434,7 +4379,7 @@
         <v>326</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -4448,7 +4393,7 @@
         <v>325</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -4459,10 +4404,10 @@
         <v>269</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -4473,7 +4418,7 @@
         <v>267</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="5.25" customHeight="1"/>
@@ -4483,10 +4428,10 @@
       </c>
       <c r="B55" s="5"/>
       <c r="D55" s="5" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G55" s="5"/>
     </row>
@@ -4498,10 +4443,10 @@
         <v>1</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="F56" s="23" t="s">
-        <v>864</v>
+        <v>776</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>863</v>
       </c>
       <c r="G56" s="6"/>
     </row>
@@ -4513,10 +4458,10 @@
         <v>0</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G57" s="6"/>
     </row>
@@ -4528,10 +4473,10 @@
         <v>0</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G58" s="6"/>
     </row>
@@ -4543,10 +4488,10 @@
         <v>0</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="F59" s="23" t="s">
-        <v>861</v>
+        <v>784</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>860</v>
       </c>
       <c r="G59" s="6"/>
     </row>
@@ -4556,7 +4501,7 @@
       </c>
       <c r="B60" s="6"/>
       <c r="D60" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -4567,7 +4512,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -4578,7 +4523,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -4589,7 +4534,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -4600,212 +4545,287 @@
         <v>0</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="6" customHeight="1"/>
-    <row r="66" spans="1:4">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="6" customHeight="1"/>
+    <row r="66" spans="1:7">
       <c r="A66" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="B66" s="5"/>
+      <c r="D66" s="21" t="s">
+        <v>788</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="B66" s="5"/>
-      <c r="D66" s="23" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="1" t="s">
+      <c r="D75" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="G75" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="1" t="s">
+      <c r="B78" s="1"/>
+      <c r="F78" s="1" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>767</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="1" t="s">
-        <v>647</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="B78" s="1"/>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="1" t="s">
-        <v>646</v>
-      </c>
       <c r="B79" s="1"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="80" spans="1:7">
+      <c r="F80" s="1" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="1" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="1" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="19" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="1" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="3" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="8" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="1" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="1" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="1" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="1" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="1" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="1" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="21" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="1" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="1" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="3" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="8" t="s">
+    <row r="94" spans="1:6">
+      <c r="A94" s="8" t="s">
         <v>698</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="8" t="s">
-        <v>699</v>
       </c>
     </row>
   </sheetData>
@@ -4825,7 +4845,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4886,7 +4906,7 @@
         <v>177</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4956,59 +4976,59 @@
         <v>581</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B10" s="5"/>
       <c r="D10" s="18" t="s">
         <v>582</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="18" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>583</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
+        <v>736</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>738</v>
-      </c>
       <c r="D12" s="18" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B13" s="5"/>
       <c r="D13" s="18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -5027,14 +5047,14 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B15" s="5"/>
       <c r="D15" s="18" t="s">
+        <v>700</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>701</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -5043,18 +5063,18 @@
       </c>
       <c r="B16" s="1"/>
       <c r="D16" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>618</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="17" spans="4:5">
       <c r="D17" s="18" t="s">
+        <v>734</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>735</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>736</v>
       </c>
     </row>
   </sheetData>
@@ -5129,22 +5149,22 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -5469,7 +5489,7 @@
   </sheetPr>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -6285,7 +6305,7 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="27" t="s">
         <v>490</v>
       </c>
     </row>
@@ -6299,7 +6319,7 @@
       <c r="E5" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
@@ -6311,7 +6331,7 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
@@ -6323,7 +6343,7 @@
       <c r="E7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
@@ -6333,7 +6353,7 @@
         <v>150</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="G8" s="26"/>
+      <c r="G8" s="27"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
@@ -6345,7 +6365,7 @@
       <c r="E9" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="G9" s="26"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
@@ -6631,7 +6651,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>368</v>
@@ -6778,7 +6798,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B35" sqref="B34:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6794,122 +6814,122 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B1" s="5"/>
       <c r="D1" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B2" s="1"/>
       <c r="D2" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>673</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>728</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="5.25" customHeight="1"/>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>388</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="5.25" customHeight="1"/>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>517</v>
@@ -6918,10 +6938,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>383</v>
@@ -6932,10 +6952,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>384</v>
@@ -6946,10 +6966,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>386</v>
@@ -6960,10 +6980,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>513</v>
@@ -6974,102 +6994,103 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B23" s="1"/>
       <c r="D23" s="6" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="E24" s="22"/>
+      <c r="E24" s="20"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="20" t="s">
+        <v>738</v>
+      </c>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="D26" s="20" t="s">
         <v>739</v>
       </c>
-      <c r="E25" s="22"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="D26" s="22" t="s">
+      <c r="E26" s="20"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="D27" s="20" t="s">
+        <v>742</v>
+      </c>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="D28" s="20" t="s">
         <v>740</v>
       </c>
-      <c r="E26" s="22"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="D27" s="22" t="s">
-        <v>743</v>
-      </c>
-      <c r="E27" s="22"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="D28" s="22" t="s">
-        <v>741</v>
-      </c>
+      <c r="E28" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7082,10 +7103,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7095,15 +7116,16 @@
     <col min="3" max="3" width="1.5703125" customWidth="1"/>
     <col min="4" max="4" width="35.28515625" customWidth="1"/>
     <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="46.5703125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>666</v>
+      <c r="B1" s="24" t="s">
+        <v>665</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>318</v>
@@ -7116,7 +7138,7 @@
       </c>
       <c r="B2" s="6"/>
       <c r="D2" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>319</v>
@@ -7130,10 +7152,10 @@
         <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>591</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -7158,7 +7180,7 @@
         <v>66</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>320</v>
@@ -7172,7 +7194,7 @@
         <v>72</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>561</v>
@@ -7186,7 +7208,7 @@
         <v>69</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -7198,53 +7220,53 @@
         <v>135</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
       <c r="D9" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>600</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>685</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>686</v>
-      </c>
       <c r="D11" s="10" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5">
       <c r="D12" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="6" t="s">
-        <v>588</v>
+      <c r="A13" s="5" t="s">
+        <v>878</v>
       </c>
       <c r="B13" s="6"/>
       <c r="D13" s="17" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -7253,10 +7275,10 @@
         <v>586</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -7266,195 +7288,204 @@
       </c>
       <c r="B15" s="1"/>
       <c r="D15" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5">
       <c r="D16" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="D17" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="5" t="s">
-        <v>560</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>562</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>824</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>610</v>
-      </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="5" t="s">
-        <v>670</v>
-      </c>
-      <c r="B20" s="6"/>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
       <c r="D20" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
-        <v>671</v>
-      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="D21" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+    </row>
+    <row r="22" spans="1:6">
       <c r="D22" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="5" t="s">
         <v>852</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
+      <c r="B24" s="6"/>
+      <c r="D24" s="5" t="s">
+        <v>875</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
+      <c r="B25" s="1"/>
+      <c r="D25" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
         <v>850</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
+      <c r="B27" s="1" t="s">
         <v>848</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
         <v>847</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
+      <c r="B28" s="1" t="s">
         <v>846</v>
       </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
+      <c r="B29" s="1" t="s">
         <v>844</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
         <v>843</v>
       </c>
+      <c r="B30" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>842</v>
-      </c>
-      <c r="B33" t="s">
-        <v>841</v>
+      <c r="A33" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>836</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>840</v>
-      </c>
-      <c r="B34" t="s">
-        <v>839</v>
+      <c r="A34" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>834</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>838</v>
-      </c>
-      <c r="B35" t="s">
-        <v>837</v>
+      <c r="A35" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>832</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>836</v>
-      </c>
-      <c r="B36" t="s">
-        <v>835</v>
+      <c r="A36" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>830</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>834</v>
-      </c>
-      <c r="B37" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>832</v>
-      </c>
-      <c r="B38" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>830</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="A37" s="1" t="s">
         <v>829</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>828</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="F24" r:id="rId2"/>
+    <hyperlink ref="F25" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -7473,33 +7504,33 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C1" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
   </sheetData>
@@ -7557,7 +7588,7 @@
         <v>514</v>
       </c>
       <c r="E12" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -7565,7 +7596,7 @@
         <v>515</v>
       </c>
       <c r="E13" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Python cheat sheet version 3.4 by Acoptex.lt
</commit_message>
<xml_diff>
--- a/python-cheatsheet-acoptexlt.xlsx
+++ b/python-cheatsheet-acoptexlt.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Barge Management\DPO\Personal\Aleksandr\PYTHON-STUFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acopt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C64821-5A91-4888-AFB9-FBE107341D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19965" yWindow="1380" windowWidth="8970" windowHeight="11850" tabRatio="803"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Various" sheetId="1" r:id="rId1"/>
@@ -17,12 +18,13 @@
     <sheet name="Data-structures" sheetId="5" r:id="rId3"/>
     <sheet name="Loops Conditions Ternary operat" sheetId="6" r:id="rId4"/>
     <sheet name="Terminal Command prompt command" sheetId="7" r:id="rId5"/>
-    <sheet name="Flask Databases" sheetId="9" r:id="rId6"/>
-    <sheet name="Modules" sheetId="4" r:id="rId7"/>
-    <sheet name="Web scrapping" sheetId="11" r:id="rId8"/>
-    <sheet name="OpenCV QT PySide " sheetId="10" r:id="rId9"/>
-    <sheet name="Links" sheetId="2" r:id="rId10"/>
-    <sheet name="Terms" sheetId="8" r:id="rId11"/>
+    <sheet name="Git_Github" sheetId="12" r:id="rId6"/>
+    <sheet name="Flask Databases" sheetId="9" r:id="rId7"/>
+    <sheet name="Modules" sheetId="4" r:id="rId8"/>
+    <sheet name="Web scrapping" sheetId="11" r:id="rId9"/>
+    <sheet name="OpenCV QT PySide " sheetId="10" r:id="rId10"/>
+    <sheet name="Links" sheetId="2" r:id="rId11"/>
+    <sheet name="Terms" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913" calcMode="autoNoTable"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="896">
   <si>
     <t>string-&gt;int</t>
   </si>
@@ -3063,9 +3065,6 @@
     <t>pip install scrapy</t>
   </si>
   <si>
-    <t>SCRAPY FRAMEWORK</t>
-  </si>
-  <si>
     <t>Beautiful soup</t>
   </si>
   <si>
@@ -3073,9 +3072,6 @@
   </si>
   <si>
     <t>pip install lxml</t>
-  </si>
-  <si>
-    <t>request libraries</t>
   </si>
   <si>
     <t>pip install requests</t>
@@ -3175,13 +3171,61 @@
     <t>parameters-&gt;when define function</t>
   </si>
   <si>
-    <t>Python Cheat Sheet version 3.3</t>
+    <t>GIT commands</t>
+  </si>
+  <si>
+    <t>git clone</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>git commit -m " "</t>
+  </si>
+  <si>
+    <t>git add file.html</t>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>Web scrapping</t>
+  </si>
+  <si>
+    <t>Required for Beautiful soup</t>
+  </si>
+  <si>
+    <t>SCRAPY framework</t>
+  </si>
+  <si>
+    <t>git push</t>
+  </si>
+  <si>
+    <t>git pull</t>
+  </si>
+  <si>
+    <t>Command creates new_branch</t>
+  </si>
+  <si>
+    <t>Command show how many branches, * shows current branch</t>
+  </si>
+  <si>
+    <t>git branch new_branch</t>
+  </si>
+  <si>
+    <t>git checkout new_branch</t>
+  </si>
+  <si>
+    <t>Command to switch to new_branch</t>
+  </si>
+  <si>
+    <t>Python Cheat Sheet version 3.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -3358,13 +3402,13 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3679,14 +3723,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3704,7 +3748,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>881</v>
+        <v>895</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -3744,7 +3788,7 @@
         <v>214</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>666</v>
@@ -3787,10 +3831,10 @@
         <v>225</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4030,7 +4074,7 @@
       <c r="B24" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="27" t="s">
         <v>743</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -4044,7 +4088,7 @@
       <c r="B25" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D25" s="26"/>
+      <c r="D25" s="27"/>
       <c r="F25" s="1" t="s">
         <v>749</v>
       </c>
@@ -4085,7 +4129,7 @@
         <v>208</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>750</v>
@@ -4099,7 +4143,7 @@
         <v>210</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>751</v>
@@ -4129,10 +4173,10 @@
         <v>677</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="I32" s="20" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -4149,7 +4193,7 @@
         <v>678</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="I33" s="20"/>
     </row>
@@ -4166,11 +4210,11 @@
       <c r="F34" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="H34" s="28" t="s">
-        <v>869</v>
+      <c r="H34" s="26" t="s">
+        <v>867</v>
       </c>
       <c r="I34" s="20" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -4393,7 +4437,7 @@
         <v>325</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -4407,7 +4451,7 @@
         <v>789</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -4431,7 +4475,7 @@
         <v>775</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="G55" s="5"/>
     </row>
@@ -4446,7 +4490,7 @@
         <v>776</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="G56" s="6"/>
     </row>
@@ -4461,7 +4505,7 @@
         <v>787</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="G57" s="6"/>
     </row>
@@ -4476,7 +4520,7 @@
         <v>777</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="G58" s="6"/>
     </row>
@@ -4491,7 +4535,7 @@
         <v>784</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="G59" s="6"/>
     </row>
@@ -4838,7 +4882,73 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="E12" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="E13" t="s">
+        <v>825</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -5080,37 +5190,37 @@
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1"/>
-    <hyperlink ref="A6" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4"/>
-    <hyperlink ref="D4" r:id="rId5"/>
-    <hyperlink ref="D5" r:id="rId6"/>
-    <hyperlink ref="D6" r:id="rId7"/>
-    <hyperlink ref="A2" r:id="rId8"/>
-    <hyperlink ref="A3" r:id="rId9"/>
-    <hyperlink ref="A4" r:id="rId10"/>
-    <hyperlink ref="D8" r:id="rId11"/>
-    <hyperlink ref="A5" r:id="rId12"/>
-    <hyperlink ref="A8" r:id="rId13"/>
-    <hyperlink ref="A7" r:id="rId14"/>
-    <hyperlink ref="D14" r:id="rId15"/>
-    <hyperlink ref="A9" r:id="rId16"/>
-    <hyperlink ref="A14" r:id="rId17"/>
-    <hyperlink ref="D10" r:id="rId18"/>
-    <hyperlink ref="D11" r:id="rId19"/>
-    <hyperlink ref="D9" r:id="rId20"/>
-    <hyperlink ref="D15" r:id="rId21"/>
-    <hyperlink ref="A11" r:id="rId22"/>
-    <hyperlink ref="D17" r:id="rId23"/>
-    <hyperlink ref="A12" r:id="rId24"/>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="A6" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
+    <hyperlink ref="A2" r:id="rId8" xr:uid="{00000000-0004-0000-0900-000007000000}"/>
+    <hyperlink ref="A3" r:id="rId9" xr:uid="{00000000-0004-0000-0900-000008000000}"/>
+    <hyperlink ref="A4" r:id="rId10" xr:uid="{00000000-0004-0000-0900-000009000000}"/>
+    <hyperlink ref="D8" r:id="rId11" xr:uid="{00000000-0004-0000-0900-00000A000000}"/>
+    <hyperlink ref="A5" r:id="rId12" xr:uid="{00000000-0004-0000-0900-00000B000000}"/>
+    <hyperlink ref="A8" r:id="rId13" xr:uid="{00000000-0004-0000-0900-00000C000000}"/>
+    <hyperlink ref="A7" r:id="rId14" xr:uid="{00000000-0004-0000-0900-00000D000000}"/>
+    <hyperlink ref="D14" r:id="rId15" xr:uid="{00000000-0004-0000-0900-00000E000000}"/>
+    <hyperlink ref="A9" r:id="rId16" xr:uid="{00000000-0004-0000-0900-00000F000000}"/>
+    <hyperlink ref="A14" r:id="rId17" xr:uid="{00000000-0004-0000-0900-000010000000}"/>
+    <hyperlink ref="D10" r:id="rId18" xr:uid="{00000000-0004-0000-0900-000011000000}"/>
+    <hyperlink ref="D11" r:id="rId19" xr:uid="{00000000-0004-0000-0900-000012000000}"/>
+    <hyperlink ref="D9" r:id="rId20" xr:uid="{00000000-0004-0000-0900-000013000000}"/>
+    <hyperlink ref="D15" r:id="rId21" xr:uid="{00000000-0004-0000-0900-000014000000}"/>
+    <hyperlink ref="A11" r:id="rId22" xr:uid="{00000000-0004-0000-0900-000015000000}"/>
+    <hyperlink ref="D17" r:id="rId23" xr:uid="{00000000-0004-0000-0900-000016000000}"/>
+    <hyperlink ref="A12" r:id="rId24" xr:uid="{00000000-0004-0000-0900-000017000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5205,7 +5315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -5483,7 +5593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -6232,14 +6342,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6305,7 +6415,7 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="28" t="s">
         <v>490</v>
       </c>
     </row>
@@ -6319,7 +6429,7 @@
       <c r="E5" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G5" s="27"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
@@ -6331,7 +6441,7 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="27"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
@@ -6343,7 +6453,7 @@
       <c r="E7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
@@ -6353,7 +6463,7 @@
         <v>150</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="G8" s="27"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
@@ -6365,7 +6475,7 @@
       <c r="E9" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="G9" s="27"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
@@ -6536,14 +6646,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6781,9 +6891,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="6.75" customHeight="1"/>
-    <row r="22" spans="1:5" ht="6" customHeight="1"/>
-    <row r="28" spans="1:5" ht="3.75" customHeight="1"/>
+    <row r="18" spans="1:5" ht="3.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6791,14 +6899,108 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F33075-4CD3-4A27-A9CF-668785147A72}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B34:B35"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7059,38 +7261,38 @@
         <v>628</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="E24" s="20"/>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>629</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="E25" s="20"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="E26" s="20"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="E27" s="20"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="E28" s="20"/>
+      <c r="E28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7098,14 +7300,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -7262,7 +7464,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B13" s="6"/>
       <c r="D13" s="17" t="s">
@@ -7360,13 +7562,13 @@
       </c>
       <c r="B24" s="6"/>
       <c r="D24" s="5" t="s">
+        <v>873</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="F24" s="18" t="s">
         <v>875</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -7480,126 +7682,72 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="F24" r:id="rId2"/>
-    <hyperlink ref="F25" r:id="rId3"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="F24" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="F25" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>859</v>
-      </c>
-      <c r="C1" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="B4" s="1" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>853</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>887</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
-        <v>391</v>
-      </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="5" t="s">
-        <v>518</v>
-      </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="E12" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="E13" t="s">
-        <v>825</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>